<commit_message>
Fixed code system URLs
</commit_message>
<xml_diff>
--- a/input/l2/WHO-ANC-mini.xlsx
+++ b/input/l2/WHO-ANC-mini.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryn\Documents\Src\WHO\smart-anc-mini\input\l2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD01309-A169-4F25-81CA-8048A7B0E69C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D77A5F-1DE8-4FC9-9A0F-83F9433B65F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="21600" windowHeight="11475" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1200" yWindow="1238" windowWidth="21600" windowHeight="11512" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="17" r:id="rId1"/>
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4263" uniqueCount="1656">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4358" uniqueCount="1656">
   <si>
     <t>Tabs</t>
   </si>
@@ -7079,9 +7079,6 @@
     <t>Encounter.location.location</t>
   </si>
   <si>
-    <t>http://fhir.org/guides/who/anc-cds/StructureDefinition/anc-observation</t>
-  </si>
-  <si>
     <t>integer quantity</t>
   </si>
   <si>
@@ -7101,12 +7098,6 @@
   </si>
   <si>
     <t>Encounter.period.start</t>
-  </si>
-  <si>
-    <t>http://fhir.org/guides/who/anc-cds/StructureDefinition/anc-base-encounter</t>
-  </si>
-  <si>
-    <t>http://fhir.org/guides/who/anc-cds/StructureDefinition/anc-base-patient</t>
   </si>
   <si>
     <t>ANC Encounter</t>
@@ -7144,9 +7135,6 @@
 ANC.A8. Validate client details</t>
   </si>
   <si>
-    <t>http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom-codes</t>
-  </si>
-  <si>
     <t>Digital adaptation kit for antenatal care: operational requirements for implementing WHO recommendations in digital systems
 Web Annex A: Core data dictionary
 NOTE: This is an excerpted version for the Mini IG to demonstrate end-to-end capability</t>
@@ -7326,13 +7314,25 @@
     <t>WHO</t>
   </si>
   <si>
-    <t>SMART-ANC-MINI</t>
-  </si>
-  <si>
-    <t>smart-anc-mini|http://fhir.org/guides/who/smart-anc-mini</t>
-  </si>
-  <si>
     <t>WHOCommon</t>
+  </si>
+  <si>
+    <t>ancm|http://fhir.org/guides/who/smart-anc-mini</t>
+  </si>
+  <si>
+    <t>ANCM</t>
+  </si>
+  <si>
+    <t>http://fhir.org/guides/who/smart-anc-mini/StructureDefinition/anc-base-patient</t>
+  </si>
+  <si>
+    <t>http://fhir.org/guides/who/smart-anc-mini/StructureDefinition/anc-base-encounter</t>
+  </si>
+  <si>
+    <t>http://fhir.org/guides/who/smart-anc-mini/StructureDefinition/anc-observation</t>
+  </si>
+  <si>
+    <t>http://fhir.org/guides/who/smart-anc-mini/CodeSystem/concept-codes</t>
   </si>
 </sst>
 </file>
@@ -15992,13 +15992,6 @@
 </externalLink>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="TAMRAT, Tigest" id="{FE507D7C-98D5-48A6-AF95-D4EDB3935476}" userId="S::tamratt@who.int::fbb8d41c-90cc-4637-8034-297d93ec23d9" providerId="AD"/>
-  <person displayName="Guy Manners (Green Ink)" id="{D673BB74-68E1-46B6-8741-DA4AD8A76268}" userId="S::g.manners@greenink.co.uk::0f72d4e3-0f22-40ba-bc66-f2cb0e17addf" providerId="AD"/>
-</personList>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -16294,29 +16287,6 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="B15" dT="2020-09-09T15:42:11.59" personId="{D673BB74-68E1-46B6-8741-DA4AD8A76268}" id="{73A4883F-312B-4EE2-B353-3877C8102745}">
-    <text>Currently blank entries to be completed by WHO or Green Ink?</text>
-  </threadedComment>
-  <threadedComment ref="B15" dT="2020-09-24T11:08:46.16" personId="{FE507D7C-98D5-48A6-AF95-D4EDB3935476}" id="{87A6F071-1EA8-4D2D-82C0-1A9E91308864}" parentId="{73A4883F-312B-4EE2-B353-3877C8102745}">
-    <text>WHO will complete</text>
-  </threadedComment>
-  <threadedComment ref="C19" dT="2020-09-16T15:04:44.74" personId="{D673BB74-68E1-46B6-8741-DA4AD8A76268}" id="{B72E0142-E372-449C-8DE0-4A24E9F40146}">
-    <text>In order for this to work, each tab will have to have exactly the same sequence of columns -- this is not currently the case</text>
-  </threadedComment>
-  <threadedComment ref="C19" dT="2020-09-24T11:11:29.44" personId="{FE507D7C-98D5-48A6-AF95-D4EDB3935476}" id="{1D061B80-FD63-4482-9B1E-A278457BDC29}" parentId="{B72E0142-E372-449C-8DE0-4A24E9F40146}">
-    <text>It should be the same columns</text>
-  </threadedComment>
-  <threadedComment ref="B21" dT="2020-09-09T15:43:01.08" personId="{D673BB74-68E1-46B6-8741-DA4AD8A76268}" id="{12303393-D127-409C-8C6F-D0999FF725C3}">
-    <text>This table is incomplete</text>
-  </threadedComment>
-  <threadedComment ref="B27" dT="2020-09-16T15:05:37.96" personId="{D673BB74-68E1-46B6-8741-DA4AD8A76268}" id="{2E84E8C4-1870-4B3E-88E3-84F2FA9969E8}">
-    <text>Perhaps need to indicate meaning of red and green texts also? Although I imagine these are for some sort of internal review reference</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A6842E-6954-44B7-9303-E97E1474C667}">
   <dimension ref="A2:K24"/>
@@ -16424,7 +16394,7 @@
     </row>
     <row r="10" spans="2:11" s="90" customFormat="1" ht="54" customHeight="1">
       <c r="B10" s="157" t="s">
-        <v>1594</v>
+        <v>1590</v>
       </c>
       <c r="C10" s="157"/>
       <c r="D10" s="157"/>
@@ -16971,10 +16941,10 @@
     <row r="34" spans="2:4" ht="42.75">
       <c r="B34" s="160"/>
       <c r="C34" s="135" t="s">
+        <v>1572</v>
+      </c>
+      <c r="D34" s="85" t="s">
         <v>1573</v>
-      </c>
-      <c r="D34" s="85" t="s">
-        <v>1574</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="57">
@@ -17463,8 +17433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16E684B6-2139-436B-862B-6D284F4F1B0E}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -17477,10 +17447,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="13.15">
       <c r="A1" s="144" t="s">
-        <v>1595</v>
+        <v>1591</v>
       </c>
       <c r="B1" s="144" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="C1" s="144" t="s">
         <v>1</v>
@@ -17488,240 +17458,240 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="146" t="s">
-        <v>1597</v>
+        <v>1593</v>
       </c>
       <c r="B2" s="146" t="s">
-        <v>1652</v>
+        <v>1648</v>
       </c>
       <c r="C2" s="146" t="s">
-        <v>1598</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="146" t="s">
-        <v>1599</v>
+        <v>1595</v>
       </c>
       <c r="B3" s="146" t="s">
-        <v>1653</v>
+        <v>1651</v>
       </c>
       <c r="C3" s="146" t="s">
-        <v>1600</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="146" t="s">
-        <v>1601</v>
+        <v>1597</v>
       </c>
       <c r="B4" s="146" t="s">
-        <v>1654</v>
+        <v>1650</v>
       </c>
       <c r="C4" s="146" t="s">
-        <v>1602</v>
+        <v>1598</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="145" t="s">
-        <v>1603</v>
+        <v>1599</v>
       </c>
       <c r="B5" s="145" t="s">
-        <v>1604</v>
+        <v>1600</v>
       </c>
       <c r="C5" s="145" t="s">
-        <v>1605</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="145" t="s">
-        <v>1606</v>
+        <v>1602</v>
       </c>
       <c r="B6" s="146" t="s">
-        <v>1607</v>
+        <v>1603</v>
       </c>
       <c r="C6" s="145" t="s">
-        <v>1608</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="145" t="s">
-        <v>1606</v>
+        <v>1602</v>
       </c>
       <c r="B7" s="146" t="s">
-        <v>1609</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="145" t="s">
-        <v>1610</v>
+        <v>1606</v>
       </c>
       <c r="B8" s="146" t="s">
-        <v>1611</v>
+        <v>1607</v>
       </c>
       <c r="C8" s="145" t="s">
-        <v>1612</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="145" t="s">
-        <v>1610</v>
+        <v>1606</v>
       </c>
       <c r="B9" s="146" t="s">
-        <v>1613</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="145" t="s">
-        <v>1614</v>
+        <v>1610</v>
       </c>
       <c r="B10" s="146" t="s">
-        <v>1615</v>
+        <v>1611</v>
       </c>
       <c r="C10" s="145" t="s">
-        <v>1616</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="145" t="s">
-        <v>1614</v>
+        <v>1610</v>
       </c>
       <c r="B11" s="146" t="s">
-        <v>1617</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="145" t="s">
-        <v>1618</v>
+        <v>1614</v>
       </c>
       <c r="B12" s="146" t="s">
-        <v>1619</v>
+        <v>1615</v>
       </c>
       <c r="C12" s="145" t="s">
-        <v>1620</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="145" t="s">
-        <v>1621</v>
+        <v>1617</v>
       </c>
       <c r="B13" s="146" t="s">
-        <v>1622</v>
+        <v>1618</v>
       </c>
       <c r="C13" s="145" t="s">
-        <v>1623</v>
+        <v>1619</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="145" t="s">
-        <v>1624</v>
+        <v>1620</v>
       </c>
       <c r="B14" s="146" t="s">
-        <v>1625</v>
+        <v>1621</v>
       </c>
       <c r="C14" s="145" t="s">
-        <v>1626</v>
+        <v>1622</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="145" t="s">
-        <v>1624</v>
+        <v>1620</v>
       </c>
       <c r="B15" s="146" t="s">
-        <v>1627</v>
+        <v>1623</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="145" t="s">
-        <v>1628</v>
+        <v>1624</v>
       </c>
       <c r="B16" s="146" t="s">
-        <v>1629</v>
+        <v>1625</v>
       </c>
       <c r="C16" s="145" t="s">
-        <v>1630</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="145" t="s">
-        <v>1631</v>
+        <v>1627</v>
       </c>
       <c r="B17" s="146" t="s">
-        <v>1632</v>
+        <v>1628</v>
       </c>
       <c r="C17" s="145" t="s">
-        <v>1633</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="145" t="s">
-        <v>1634</v>
+        <v>1630</v>
       </c>
       <c r="B18" s="146" t="s">
-        <v>1635</v>
+        <v>1631</v>
       </c>
       <c r="C18" s="145" t="s">
-        <v>1636</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="145" t="s">
-        <v>1637</v>
+        <v>1633</v>
       </c>
       <c r="B19" s="146" t="s">
-        <v>1638</v>
+        <v>1634</v>
       </c>
       <c r="C19" s="145" t="s">
-        <v>1639</v>
+        <v>1635</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="145" t="s">
-        <v>1637</v>
+        <v>1633</v>
       </c>
       <c r="B20" s="146" t="s">
-        <v>1640</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="145" t="s">
-        <v>1641</v>
+        <v>1637</v>
       </c>
       <c r="B21" s="146" t="s">
-        <v>1642</v>
+        <v>1638</v>
       </c>
       <c r="C21" s="145" t="s">
-        <v>1643</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="145" t="s">
-        <v>1644</v>
+        <v>1640</v>
       </c>
       <c r="B22" s="146" t="s">
-        <v>1645</v>
+        <v>1641</v>
       </c>
       <c r="C22" s="145" t="s">
-        <v>1646</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="145" t="s">
-        <v>1647</v>
+        <v>1643</v>
       </c>
       <c r="B23" s="146" t="s">
-        <v>1648</v>
+        <v>1644</v>
       </c>
       <c r="C23" s="145" t="s">
-        <v>1649</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="145" t="s">
-        <v>1650</v>
+        <v>1646</v>
       </c>
       <c r="B24" s="145" t="s">
-        <v>1655</v>
+        <v>1649</v>
       </c>
       <c r="C24" s="145" t="s">
-        <v>1651</v>
+        <v>1647</v>
       </c>
     </row>
   </sheetData>
@@ -17738,10 +17708,10 @@
   <dimension ref="B1:AV25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="AJ3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AO7" sqref="AO7"/>
+      <selection pane="bottomRight" activeCell="AR26" sqref="AR26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="13.15"/>
@@ -17932,10 +17902,10 @@
         <v>151</v>
       </c>
       <c r="AP2" s="127" t="s">
+        <v>1581</v>
+      </c>
+      <c r="AQ2" s="127" t="s">
         <v>1584</v>
-      </c>
-      <c r="AQ2" s="127" t="s">
-        <v>1587</v>
       </c>
       <c r="AR2" s="127" t="s">
         <v>152</v>
@@ -17955,7 +17925,7 @@
     </row>
     <row r="3" spans="2:48" ht="30" customHeight="1">
       <c r="B3" s="34" t="s">
-        <v>1591</v>
+        <v>1588</v>
       </c>
       <c r="C3" s="104" t="s">
         <v>168</v>
@@ -18025,21 +17995,24 @@
         <v>177</v>
       </c>
       <c r="AI3" s="140" t="s">
-        <v>1581</v>
+        <v>1652</v>
       </c>
       <c r="AJ3" s="29" t="s">
         <v>165</v>
       </c>
       <c r="AL3" s="29" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="AO3" s="29" t="s">
-        <v>1653</v>
+        <v>1651</v>
+      </c>
+      <c r="AR3" s="132" t="s">
+        <v>1655</v>
       </c>
     </row>
     <row r="4" spans="2:48" ht="30" customHeight="1">
       <c r="B4" s="34" t="s">
-        <v>1591</v>
+        <v>1588</v>
       </c>
       <c r="C4" s="104" t="s">
         <v>178</v>
@@ -18111,21 +18084,24 @@
         <v>177</v>
       </c>
       <c r="AI4" s="140" t="s">
-        <v>1581</v>
+        <v>1652</v>
       </c>
       <c r="AJ4" s="29" t="s">
         <v>165</v>
       </c>
       <c r="AL4" s="29" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="AO4" s="29" t="s">
-        <v>1653</v>
+        <v>1651</v>
+      </c>
+      <c r="AR4" s="132" t="s">
+        <v>1655</v>
       </c>
     </row>
     <row r="5" spans="2:48" ht="30" customHeight="1">
       <c r="B5" s="34" t="s">
-        <v>1591</v>
+        <v>1588</v>
       </c>
       <c r="C5" s="104" t="s">
         <v>187</v>
@@ -18197,21 +18173,24 @@
         <v>177</v>
       </c>
       <c r="AI5" s="140" t="s">
-        <v>1581</v>
+        <v>1652</v>
       </c>
       <c r="AJ5" s="29" t="s">
         <v>165</v>
       </c>
       <c r="AL5" s="29" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="AO5" s="29" t="s">
-        <v>1653</v>
+        <v>1651</v>
+      </c>
+      <c r="AR5" s="132" t="s">
+        <v>1655</v>
       </c>
     </row>
     <row r="6" spans="2:48" s="16" customFormat="1" ht="30" customHeight="1">
       <c r="B6" s="34" t="s">
-        <v>1591</v>
+        <v>1588</v>
       </c>
       <c r="C6" s="104" t="s">
         <v>196</v>
@@ -18282,33 +18261,36 @@
         <v>205</v>
       </c>
       <c r="AF6" s="16" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="AG6" s="16" t="s">
         <v>164</v>
       </c>
       <c r="AI6" s="140" t="s">
-        <v>1580</v>
+        <v>1653</v>
       </c>
       <c r="AJ6" s="29" t="s">
         <v>165</v>
       </c>
       <c r="AL6" s="29" t="s">
+        <v>1579</v>
+      </c>
+      <c r="AO6" s="29" t="s">
+        <v>1651</v>
+      </c>
+      <c r="AP6" s="16" t="s">
         <v>1582</v>
       </c>
-      <c r="AO6" s="29" t="s">
-        <v>1653</v>
-      </c>
-      <c r="AP6" s="16" t="s">
-        <v>1585</v>
-      </c>
       <c r="AQ6" s="16" t="s">
-        <v>1586</v>
+        <v>1583</v>
+      </c>
+      <c r="AR6" s="132" t="s">
+        <v>1655</v>
       </c>
     </row>
     <row r="7" spans="2:48" ht="30" customHeight="1">
       <c r="B7" s="34" t="s">
-        <v>1592</v>
+        <v>1589</v>
       </c>
       <c r="C7" s="104" t="s">
         <v>207</v>
@@ -18381,21 +18363,24 @@
         <v>164</v>
       </c>
       <c r="AI7" s="140" t="s">
-        <v>1581</v>
+        <v>1652</v>
       </c>
       <c r="AJ7" s="29" t="s">
         <v>165</v>
       </c>
       <c r="AL7" s="29" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="AO7" s="29" t="s">
-        <v>1653</v>
+        <v>1651</v>
+      </c>
+      <c r="AR7" s="132" t="s">
+        <v>1655</v>
       </c>
     </row>
     <row r="8" spans="2:48" ht="30" customHeight="1">
       <c r="B8" s="34" t="s">
-        <v>1592</v>
+        <v>1589</v>
       </c>
       <c r="C8" s="104" t="s">
         <v>215</v>
@@ -18463,6 +18448,12 @@
       </c>
       <c r="AD8" s="28" t="s">
         <v>226</v>
+      </c>
+      <c r="AO8" s="29" t="s">
+        <v>1651</v>
+      </c>
+      <c r="AR8" s="132" t="s">
+        <v>1655</v>
       </c>
     </row>
     <row r="9" spans="2:48" ht="30" customHeight="1">
@@ -18664,16 +18655,19 @@
         <v>177</v>
       </c>
       <c r="AI13" s="29" t="s">
-        <v>1581</v>
+        <v>1652</v>
       </c>
       <c r="AJ13" s="29" t="s">
         <v>165</v>
       </c>
       <c r="AL13" s="29" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="AO13" s="29" t="s">
-        <v>166</v>
+        <v>1651</v>
+      </c>
+      <c r="AR13" s="132" t="s">
+        <v>1655</v>
       </c>
     </row>
     <row r="14" spans="2:48" ht="30" customHeight="1">
@@ -18698,7 +18692,7 @@
       <c r="H14" s="26"/>
       <c r="I14" s="26"/>
       <c r="J14" s="26" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
       <c r="K14" s="26" t="s">
         <v>157</v>
@@ -18748,16 +18742,19 @@
         <v>177</v>
       </c>
       <c r="AI14" s="130" t="s">
-        <v>1581</v>
+        <v>1652</v>
       </c>
       <c r="AJ14" s="130" t="s">
         <v>165</v>
       </c>
       <c r="AL14" s="29" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="AO14" s="29" t="s">
-        <v>166</v>
+        <v>1651</v>
+      </c>
+      <c r="AR14" s="132" t="s">
+        <v>1655</v>
       </c>
     </row>
     <row r="15" spans="2:48" ht="30" customHeight="1">
@@ -18832,7 +18829,7 @@
         <v>263</v>
       </c>
       <c r="AF15" s="29" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="AG15" s="29" t="s">
         <v>264</v>
@@ -18841,16 +18838,19 @@
         <v>158</v>
       </c>
       <c r="AI15" s="130" t="s">
-        <v>1581</v>
+        <v>1652</v>
       </c>
       <c r="AJ15" s="29" t="s">
         <v>165</v>
       </c>
       <c r="AL15" s="29" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="AO15" s="29" t="s">
-        <v>166</v>
+        <v>1651</v>
+      </c>
+      <c r="AR15" s="132" t="s">
+        <v>1655</v>
       </c>
     </row>
     <row r="16" spans="2:48" ht="30" customHeight="1">
@@ -18925,16 +18925,19 @@
         <v>177</v>
       </c>
       <c r="AI16" s="130" t="s">
-        <v>1581</v>
+        <v>1652</v>
       </c>
       <c r="AJ16" s="130" t="s">
         <v>165</v>
       </c>
       <c r="AL16" s="29" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="AO16" s="29" t="s">
-        <v>166</v>
+        <v>1651</v>
+      </c>
+      <c r="AR16" s="132" t="s">
+        <v>1655</v>
       </c>
     </row>
     <row r="17" spans="2:44" ht="30" customHeight="1">
@@ -18959,7 +18962,7 @@
       <c r="H17" s="26"/>
       <c r="I17" s="26"/>
       <c r="J17" s="26" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
       <c r="K17" s="26" t="s">
         <v>157</v>
@@ -19009,16 +19012,19 @@
         <v>177</v>
       </c>
       <c r="AI17" s="130" t="s">
-        <v>1581</v>
+        <v>1652</v>
       </c>
       <c r="AJ17" s="130" t="s">
         <v>165</v>
       </c>
       <c r="AL17" s="29" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="AO17" s="29" t="s">
-        <v>166</v>
+        <v>1651</v>
+      </c>
+      <c r="AR17" s="132" t="s">
+        <v>1655</v>
       </c>
     </row>
     <row r="18" spans="2:44" ht="30" customHeight="1">
@@ -19043,7 +19049,7 @@
       <c r="H18" s="26"/>
       <c r="I18" s="26"/>
       <c r="J18" s="26" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
       <c r="K18" s="26" t="s">
         <v>157</v>
@@ -19087,31 +19093,34 @@
         <v>285</v>
       </c>
       <c r="AF18" s="29" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="AG18" s="29" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="AH18" s="29" t="s">
         <v>158</v>
       </c>
       <c r="AI18" s="143" t="s">
-        <v>1580</v>
+        <v>1653</v>
       </c>
       <c r="AJ18" s="130" t="s">
         <v>165</v>
       </c>
       <c r="AL18" s="29" t="s">
+        <v>1579</v>
+      </c>
+      <c r="AO18" s="29" t="s">
+        <v>1651</v>
+      </c>
+      <c r="AP18" s="29" t="s">
         <v>1582</v>
       </c>
-      <c r="AO18" s="29" t="s">
-        <v>166</v>
-      </c>
-      <c r="AP18" s="29" t="s">
-        <v>1585</v>
-      </c>
       <c r="AQ18" s="29" t="s">
-        <v>1586</v>
+        <v>1583</v>
+      </c>
+      <c r="AR18" s="132" t="s">
+        <v>1655</v>
       </c>
     </row>
     <row r="19" spans="2:44" s="51" customFormat="1" ht="30" customHeight="1">
@@ -19160,16 +19169,16 @@
         <v>290</v>
       </c>
       <c r="AI19" s="131" t="s">
-        <v>1572</v>
+        <v>1654</v>
       </c>
       <c r="AJ19" s="51" t="s">
         <v>165</v>
       </c>
-      <c r="AO19" s="51" t="s">
-        <v>166</v>
+      <c r="AO19" s="29" t="s">
+        <v>1651</v>
       </c>
       <c r="AR19" s="132" t="s">
-        <v>1593</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="20" spans="2:44" s="28" customFormat="1" ht="30" customHeight="1">
@@ -19240,8 +19249,11 @@
       <c r="AJ20" s="130" t="s">
         <v>165</v>
       </c>
-      <c r="AO20" s="28" t="s">
-        <v>166</v>
+      <c r="AO20" s="29" t="s">
+        <v>1651</v>
+      </c>
+      <c r="AR20" s="132" t="s">
+        <v>1655</v>
       </c>
     </row>
     <row r="21" spans="2:44" s="28" customFormat="1" ht="30" customHeight="1">
@@ -19311,8 +19323,11 @@
       <c r="AJ21" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="AO21" s="28" t="s">
-        <v>166</v>
+      <c r="AO21" s="29" t="s">
+        <v>1651</v>
+      </c>
+      <c r="AR21" s="132" t="s">
+        <v>1655</v>
       </c>
     </row>
     <row r="22" spans="2:44" s="28" customFormat="1" ht="30" customHeight="1">
@@ -19382,8 +19397,11 @@
       <c r="AJ22" s="130" t="s">
         <v>165</v>
       </c>
-      <c r="AO22" s="28" t="s">
-        <v>166</v>
+      <c r="AO22" s="29" t="s">
+        <v>1651</v>
+      </c>
+      <c r="AR22" s="132" t="s">
+        <v>1655</v>
       </c>
     </row>
     <row r="23" spans="2:44" s="28" customFormat="1" ht="30" customHeight="1">
@@ -19456,8 +19474,11 @@
       <c r="AJ23" s="130" t="s">
         <v>165</v>
       </c>
-      <c r="AO23" s="28" t="s">
-        <v>166</v>
+      <c r="AO23" s="29" t="s">
+        <v>1651</v>
+      </c>
+      <c r="AR23" s="132" t="s">
+        <v>1655</v>
       </c>
     </row>
     <row r="24" spans="2:44" s="28" customFormat="1" ht="30" customHeight="1">
@@ -19530,8 +19551,11 @@
       <c r="AJ24" s="130" t="s">
         <v>165</v>
       </c>
-      <c r="AO24" s="28" t="s">
-        <v>166</v>
+      <c r="AO24" s="29" t="s">
+        <v>1651</v>
+      </c>
+      <c r="AR24" s="132" t="s">
+        <v>1655</v>
       </c>
     </row>
     <row r="25" spans="2:44" s="28" customFormat="1" ht="30" customHeight="1">
@@ -19601,8 +19625,11 @@
       <c r="AJ25" s="28" t="s">
         <v>165</v>
       </c>
-      <c r="AO25" s="28" t="s">
-        <v>166</v>
+      <c r="AO25" s="29" t="s">
+        <v>1651</v>
+      </c>
+      <c r="AR25" s="132" t="s">
+        <v>1655</v>
       </c>
     </row>
   </sheetData>
@@ -19617,16 +19644,34 @@
     <hyperlink ref="R8" r:id="rId1" xr:uid="{6C6A1B00-41B0-4F3D-8429-8336E8F2A6EC}"/>
     <hyperlink ref="AI19" r:id="rId2" display="http://fhir.org/guides/who/anc-cds/StructureDefinition/who-observation" xr:uid="{2D11DB1F-B495-E74D-8209-A54BC0E4DB95}"/>
     <hyperlink ref="AR19" r:id="rId3" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{D5324F85-2DDF-E14C-A7B6-AD4890DCC987}"/>
-    <hyperlink ref="AI18" r:id="rId4" xr:uid="{F8FE929C-1B1E-4A44-BFD8-A582869F333E}"/>
-    <hyperlink ref="AI3" r:id="rId5" xr:uid="{FA0C751A-4585-4164-893A-0D01A170D2DC}"/>
-    <hyperlink ref="AI4" r:id="rId6" xr:uid="{CCF83D7E-7772-4A36-8539-AAF4D1F54578}"/>
-    <hyperlink ref="AI5" r:id="rId7" xr:uid="{1425C138-5CC1-40CD-850B-CA0AE001E2DB}"/>
-    <hyperlink ref="AI6" r:id="rId8" xr:uid="{1C06BFA9-5880-417C-928C-AA85A52D843C}"/>
-    <hyperlink ref="AI7" r:id="rId9" xr:uid="{E40713C1-1F3B-405C-A520-AC96D65D62DF}"/>
+    <hyperlink ref="AI18" r:id="rId4" display="http://fhir.org/guides/who/anc-cds/StructureDefinition/anc-base-encounter" xr:uid="{F8FE929C-1B1E-4A44-BFD8-A582869F333E}"/>
+    <hyperlink ref="AI3" r:id="rId5" display="http://fhir.org/guides/who/anc-cds/StructureDefinition/anc-base-patient" xr:uid="{FA0C751A-4585-4164-893A-0D01A170D2DC}"/>
+    <hyperlink ref="AI4" r:id="rId6" display="http://fhir.org/guides/who/anc-cds/StructureDefinition/anc-base-patient" xr:uid="{CCF83D7E-7772-4A36-8539-AAF4D1F54578}"/>
+    <hyperlink ref="AI5" r:id="rId7" display="http://fhir.org/guides/who/anc-cds/StructureDefinition/anc-base-patient" xr:uid="{1425C138-5CC1-40CD-850B-CA0AE001E2DB}"/>
+    <hyperlink ref="AI6" r:id="rId8" display="http://fhir.org/guides/who/anc-cds/StructureDefinition/anc-base-encounter" xr:uid="{1C06BFA9-5880-417C-928C-AA85A52D843C}"/>
+    <hyperlink ref="AI7" r:id="rId9" display="http://fhir.org/guides/who/anc-cds/StructureDefinition/anc-base-patient" xr:uid="{E40713C1-1F3B-405C-A520-AC96D65D62DF}"/>
+    <hyperlink ref="AR3" r:id="rId10" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{53A41483-7481-439D-B8A7-E237489685A7}"/>
+    <hyperlink ref="AR4" r:id="rId11" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{B95EE22A-548A-4969-90CD-8189A7A793E7}"/>
+    <hyperlink ref="AR5" r:id="rId12" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{7D5E7634-D81F-4AAF-9198-C16E4AE47299}"/>
+    <hyperlink ref="AR6" r:id="rId13" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{90524CBD-34A6-448C-80BF-ACB041329581}"/>
+    <hyperlink ref="AR7" r:id="rId14" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{7EB3D25F-030D-486E-8293-268FBF92426F}"/>
+    <hyperlink ref="AR8" r:id="rId15" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{0843F5DA-565E-4092-98E0-A47324150B99}"/>
+    <hyperlink ref="AR13" r:id="rId16" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{50521937-C066-41A3-B7C4-5CA02F1BB0B3}"/>
+    <hyperlink ref="AR14" r:id="rId17" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{AE2C3D19-111D-405A-A1BC-A69DE88D4A58}"/>
+    <hyperlink ref="AR15" r:id="rId18" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{51D29041-6667-4CF8-AE2F-E3D46A247A2F}"/>
+    <hyperlink ref="AR16" r:id="rId19" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{F8747797-71F2-4544-B1C1-7D97DEF35A91}"/>
+    <hyperlink ref="AR17" r:id="rId20" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{5A698461-FC20-4D82-9B06-0338F4226448}"/>
+    <hyperlink ref="AR18" r:id="rId21" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{EAFC68A3-1778-4B07-8FE7-0EC05C6CCEB6}"/>
+    <hyperlink ref="AR20" r:id="rId22" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{184E889F-DF73-4079-A2F5-D17720A4C877}"/>
+    <hyperlink ref="AR21" r:id="rId23" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{A111079F-915F-48E1-B0B9-AF7BC5651763}"/>
+    <hyperlink ref="AR22" r:id="rId24" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{E4C0EB20-1450-4FED-9067-5EF96A980D09}"/>
+    <hyperlink ref="AR23" r:id="rId25" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{61FFEEE5-4354-47A4-94A9-76FE4A9632FB}"/>
+    <hyperlink ref="AR24" r:id="rId26" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{25072E2D-829A-46CD-AA22-B4C0C3076E2C}"/>
+    <hyperlink ref="AR25" r:id="rId27" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{3F3216EC-5507-4F8A-99B2-8A706114A9E6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId10"/>
-  <drawing r:id="rId11"/>
+  <pageSetup orientation="landscape" r:id="rId28"/>
+  <drawing r:id="rId29"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
@@ -19674,10 +19719,10 @@
   <dimension ref="B1:AY65"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="7" ySplit="2" topLeftCell="AP58" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="2" topLeftCell="AT58" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AR65" sqref="AR65"/>
+      <selection pane="bottomRight" activeCell="AU64" sqref="AU64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="13.15"/>
@@ -19890,10 +19935,10 @@
         <v>151</v>
       </c>
       <c r="AS2" s="127" t="s">
+        <v>1581</v>
+      </c>
+      <c r="AT2" s="127" t="s">
         <v>1584</v>
-      </c>
-      <c r="AT2" s="127" t="s">
-        <v>1587</v>
       </c>
       <c r="AU2" s="127" t="s">
         <v>152</v>
@@ -19994,7 +20039,7 @@
       </c>
       <c r="AK3" s="119"/>
       <c r="AL3" t="s">
-        <v>1572</v>
+        <v>1654</v>
       </c>
       <c r="AM3" s="119" t="s">
         <v>165</v>
@@ -20004,16 +20049,16 @@
       <c r="AP3"/>
       <c r="AQ3"/>
       <c r="AR3" s="119" t="s">
-        <v>166</v>
+        <v>1651</v>
       </c>
       <c r="AS3" s="119" t="s">
-        <v>1585</v>
+        <v>1582</v>
       </c>
       <c r="AT3" s="119" t="s">
-        <v>1586</v>
+        <v>1583</v>
       </c>
       <c r="AU3" s="132" t="s">
-        <v>1593</v>
+        <v>1655</v>
       </c>
       <c r="AV3"/>
     </row>
@@ -20087,28 +20132,28 @@
       </c>
       <c r="AK4"/>
       <c r="AL4" s="141" t="s">
-        <v>1580</v>
+        <v>1653</v>
       </c>
       <c r="AM4" s="119" t="s">
         <v>165</v>
       </c>
       <c r="AN4"/>
       <c r="AO4" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="AP4"/>
       <c r="AQ4"/>
       <c r="AR4" s="119" t="s">
-        <v>166</v>
+        <v>1651</v>
       </c>
       <c r="AS4" s="119" t="s">
-        <v>1585</v>
+        <v>1582</v>
       </c>
       <c r="AT4" s="119" t="s">
-        <v>1586</v>
+        <v>1583</v>
       </c>
       <c r="AU4" s="132" t="s">
-        <v>1593</v>
+        <v>1655</v>
       </c>
       <c r="AV4"/>
     </row>
@@ -20202,15 +20247,17 @@
       <c r="AN5"/>
       <c r="AO5"/>
       <c r="AP5" t="s">
-        <v>1589</v>
+        <v>1586</v>
       </c>
       <c r="AQ5"/>
-      <c r="AR5" s="73" t="s">
-        <v>166</v>
+      <c r="AR5" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS5" s="73"/>
       <c r="AT5" s="73"/>
-      <c r="AU5"/>
+      <c r="AU5" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV5"/>
     </row>
     <row r="6" spans="2:51" ht="30" customHeight="1">
@@ -20301,15 +20348,17 @@
       <c r="AN6"/>
       <c r="AO6"/>
       <c r="AP6" t="s">
-        <v>1590</v>
+        <v>1587</v>
       </c>
       <c r="AQ6"/>
-      <c r="AR6" s="73" t="s">
-        <v>166</v>
+      <c r="AR6" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS6" s="73"/>
       <c r="AT6" s="73"/>
-      <c r="AU6"/>
+      <c r="AU6" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV6"/>
     </row>
     <row r="7" spans="2:51" ht="30" customHeight="1">
@@ -20401,12 +20450,14 @@
       <c r="AO7"/>
       <c r="AP7"/>
       <c r="AQ7"/>
-      <c r="AR7" s="73" t="s">
-        <v>166</v>
+      <c r="AR7" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS7" s="73"/>
       <c r="AT7" s="73"/>
-      <c r="AU7"/>
+      <c r="AU7" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV7"/>
     </row>
     <row r="8" spans="2:51" s="55" customFormat="1" ht="30" customHeight="1">
@@ -20482,7 +20533,7 @@
       </c>
       <c r="AK8" s="119"/>
       <c r="AL8" t="s">
-        <v>1572</v>
+        <v>1654</v>
       </c>
       <c r="AM8" s="119" t="s">
         <v>165</v>
@@ -20491,15 +20542,15 @@
       <c r="AO8"/>
       <c r="AP8"/>
       <c r="AQ8"/>
-      <c r="AR8" s="73" t="s">
-        <v>166</v>
+      <c r="AR8" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS8" s="73" t="s">
-        <v>1585</v>
+        <v>1582</v>
       </c>
       <c r="AT8" s="73"/>
       <c r="AU8" s="132" t="s">
-        <v>1593</v>
+        <v>1655</v>
       </c>
       <c r="AV8" s="50"/>
       <c r="AW8" s="50"/>
@@ -20602,11 +20653,13 @@
       <c r="AP9"/>
       <c r="AQ9"/>
       <c r="AR9" s="119" t="s">
-        <v>166</v>
+        <v>1651</v>
       </c>
       <c r="AS9" s="119"/>
       <c r="AT9" s="119"/>
-      <c r="AU9"/>
+      <c r="AU9" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV9"/>
     </row>
     <row r="10" spans="2:51" ht="30" customHeight="1">
@@ -20705,11 +20758,13 @@
       <c r="AP10"/>
       <c r="AQ10"/>
       <c r="AR10" s="119" t="s">
-        <v>166</v>
+        <v>1651</v>
       </c>
       <c r="AS10" s="119"/>
       <c r="AT10" s="119"/>
-      <c r="AU10"/>
+      <c r="AU10" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV10"/>
     </row>
     <row r="11" spans="2:51" ht="30" customHeight="1">
@@ -20807,12 +20862,14 @@
       <c r="AO11"/>
       <c r="AP11"/>
       <c r="AQ11"/>
-      <c r="AR11" s="73" t="s">
-        <v>166</v>
+      <c r="AR11" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS11" s="73"/>
       <c r="AT11" s="73"/>
-      <c r="AU11"/>
+      <c r="AU11" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV11"/>
     </row>
     <row r="12" spans="2:51" ht="30" customHeight="1">
@@ -20912,12 +20969,14 @@
       <c r="AO12"/>
       <c r="AP12"/>
       <c r="AQ12"/>
-      <c r="AR12" s="73" t="s">
-        <v>166</v>
+      <c r="AR12" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS12" s="73"/>
       <c r="AT12" s="73"/>
-      <c r="AU12"/>
+      <c r="AU12" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV12"/>
     </row>
     <row r="13" spans="2:51" ht="30" customHeight="1">
@@ -21017,12 +21076,14 @@
       <c r="AO13"/>
       <c r="AP13"/>
       <c r="AQ13"/>
-      <c r="AR13" s="73" t="s">
-        <v>166</v>
+      <c r="AR13" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS13" s="73"/>
       <c r="AT13" s="73"/>
-      <c r="AU13"/>
+      <c r="AU13" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV13"/>
     </row>
     <row r="14" spans="2:51" ht="30" customHeight="1">
@@ -21122,12 +21183,14 @@
       <c r="AO14"/>
       <c r="AP14"/>
       <c r="AQ14"/>
-      <c r="AR14" s="73" t="s">
-        <v>166</v>
+      <c r="AR14" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS14" s="73"/>
       <c r="AT14" s="73"/>
-      <c r="AU14"/>
+      <c r="AU14" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV14"/>
     </row>
     <row r="15" spans="2:51" ht="30" customHeight="1">
@@ -21222,11 +21285,13 @@
       <c r="AP15"/>
       <c r="AQ15"/>
       <c r="AR15" s="119" t="s">
-        <v>166</v>
+        <v>1651</v>
       </c>
       <c r="AS15" s="119"/>
       <c r="AT15" s="119"/>
-      <c r="AU15"/>
+      <c r="AU15" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV15"/>
     </row>
     <row r="16" spans="2:51" ht="30" customHeight="1">
@@ -21327,11 +21392,13 @@
       <c r="AP16"/>
       <c r="AQ16"/>
       <c r="AR16" s="119" t="s">
-        <v>166</v>
+        <v>1651</v>
       </c>
       <c r="AS16" s="119"/>
       <c r="AT16" s="119"/>
-      <c r="AU16"/>
+      <c r="AU16" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV16"/>
     </row>
     <row r="17" spans="2:48" ht="30" customHeight="1">
@@ -21429,12 +21496,14 @@
       <c r="AO17"/>
       <c r="AP17"/>
       <c r="AQ17"/>
-      <c r="AR17" s="73" t="s">
-        <v>166</v>
+      <c r="AR17" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS17" s="73"/>
       <c r="AT17" s="73"/>
-      <c r="AU17"/>
+      <c r="AU17" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV17"/>
     </row>
     <row r="18" spans="2:48" ht="30" customHeight="1">
@@ -21530,12 +21599,14 @@
       <c r="AO18"/>
       <c r="AP18"/>
       <c r="AQ18"/>
-      <c r="AR18" s="73" t="s">
-        <v>166</v>
+      <c r="AR18" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS18" s="73"/>
       <c r="AT18" s="73"/>
-      <c r="AU18"/>
+      <c r="AU18" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV18"/>
     </row>
     <row r="19" spans="2:48" ht="30" customHeight="1">
@@ -21631,12 +21702,14 @@
       <c r="AO19"/>
       <c r="AP19"/>
       <c r="AQ19"/>
-      <c r="AR19" s="73" t="s">
-        <v>166</v>
+      <c r="AR19" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS19" s="73"/>
       <c r="AT19" s="73"/>
-      <c r="AU19"/>
+      <c r="AU19" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV19"/>
     </row>
     <row r="20" spans="2:48" ht="30" customHeight="1">
@@ -21734,12 +21807,14 @@
       <c r="AO20"/>
       <c r="AP20"/>
       <c r="AQ20"/>
-      <c r="AR20" s="73" t="s">
-        <v>166</v>
+      <c r="AR20" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS20" s="73"/>
       <c r="AT20" s="73"/>
-      <c r="AU20"/>
+      <c r="AU20" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV20"/>
     </row>
     <row r="21" spans="2:48" ht="30" customHeight="1">
@@ -21838,11 +21913,13 @@
       <c r="AP21"/>
       <c r="AQ21"/>
       <c r="AR21" s="119" t="s">
-        <v>166</v>
+        <v>1651</v>
       </c>
       <c r="AS21" s="119"/>
       <c r="AT21" s="119"/>
-      <c r="AU21"/>
+      <c r="AU21" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV21"/>
     </row>
     <row r="22" spans="2:48" ht="30" customHeight="1">
@@ -21939,11 +22016,13 @@
       <c r="AP22"/>
       <c r="AQ22"/>
       <c r="AR22" s="119" t="s">
-        <v>166</v>
+        <v>1651</v>
       </c>
       <c r="AS22" s="119"/>
       <c r="AT22" s="119"/>
-      <c r="AU22"/>
+      <c r="AU22" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV22"/>
     </row>
     <row r="23" spans="2:48" ht="30" customHeight="1">
@@ -22041,12 +22120,14 @@
       <c r="AO23"/>
       <c r="AP23"/>
       <c r="AQ23"/>
-      <c r="AR23" s="73" t="s">
-        <v>166</v>
+      <c r="AR23" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS23" s="73"/>
       <c r="AT23" s="73"/>
-      <c r="AU23"/>
+      <c r="AU23" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV23"/>
     </row>
     <row r="24" spans="2:48" ht="30" customHeight="1">
@@ -22146,12 +22227,14 @@
       <c r="AO24"/>
       <c r="AP24"/>
       <c r="AQ24"/>
-      <c r="AR24" s="73" t="s">
-        <v>166</v>
+      <c r="AR24" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS24" s="73"/>
       <c r="AT24" s="73"/>
-      <c r="AU24"/>
+      <c r="AU24" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV24"/>
     </row>
     <row r="25" spans="2:48" ht="30" customHeight="1">
@@ -22249,12 +22332,14 @@
       <c r="AO25"/>
       <c r="AP25"/>
       <c r="AQ25"/>
-      <c r="AR25" s="73" t="s">
-        <v>166</v>
+      <c r="AR25" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS25" s="73"/>
       <c r="AT25" s="73"/>
-      <c r="AU25"/>
+      <c r="AU25" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV25"/>
     </row>
     <row r="26" spans="2:48" ht="30" customHeight="1">
@@ -22350,12 +22435,14 @@
       <c r="AO26"/>
       <c r="AP26"/>
       <c r="AQ26"/>
-      <c r="AR26" s="73" t="s">
-        <v>166</v>
+      <c r="AR26" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS26" s="73"/>
       <c r="AT26" s="73"/>
-      <c r="AU26"/>
+      <c r="AU26" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV26"/>
     </row>
     <row r="27" spans="2:48" ht="30" customHeight="1">
@@ -22454,11 +22541,13 @@
       <c r="AP27"/>
       <c r="AQ27"/>
       <c r="AR27" s="119" t="s">
-        <v>166</v>
+        <v>1651</v>
       </c>
       <c r="AS27" s="119"/>
       <c r="AT27" s="119"/>
-      <c r="AU27"/>
+      <c r="AU27" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV27"/>
     </row>
     <row r="28" spans="2:48" ht="30" customHeight="1">
@@ -22557,11 +22646,13 @@
       <c r="AP28"/>
       <c r="AQ28"/>
       <c r="AR28" s="119" t="s">
-        <v>166</v>
+        <v>1651</v>
       </c>
       <c r="AS28" s="119"/>
       <c r="AT28" s="119"/>
-      <c r="AU28"/>
+      <c r="AU28" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV28"/>
     </row>
     <row r="29" spans="2:48" ht="30" customHeight="1">
@@ -22661,12 +22752,14 @@
       <c r="AO29"/>
       <c r="AP29"/>
       <c r="AQ29"/>
-      <c r="AR29" s="73" t="s">
-        <v>166</v>
+      <c r="AR29" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS29" s="73"/>
       <c r="AT29" s="73"/>
-      <c r="AU29"/>
+      <c r="AU29" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV29"/>
     </row>
     <row r="30" spans="2:48" ht="30" customHeight="1">
@@ -22764,12 +22857,14 @@
       <c r="AO30"/>
       <c r="AP30"/>
       <c r="AQ30"/>
-      <c r="AR30" s="73" t="s">
-        <v>166</v>
+      <c r="AR30" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS30" s="73"/>
       <c r="AT30" s="73"/>
-      <c r="AU30"/>
+      <c r="AU30" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV30"/>
     </row>
     <row r="31" spans="2:48" ht="30" customHeight="1">
@@ -22869,12 +22964,14 @@
       <c r="AO31"/>
       <c r="AP31"/>
       <c r="AQ31"/>
-      <c r="AR31" s="73" t="s">
-        <v>166</v>
+      <c r="AR31" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS31" s="73"/>
       <c r="AT31" s="73"/>
-      <c r="AU31"/>
+      <c r="AU31" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV31"/>
     </row>
     <row r="32" spans="2:48" ht="30" customHeight="1">
@@ -22974,12 +23071,14 @@
       <c r="AO32"/>
       <c r="AP32"/>
       <c r="AQ32"/>
-      <c r="AR32" s="73" t="s">
-        <v>166</v>
+      <c r="AR32" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS32" s="73"/>
       <c r="AT32" s="73"/>
-      <c r="AU32"/>
+      <c r="AU32" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV32"/>
     </row>
     <row r="33" spans="2:48" ht="30" customHeight="1">
@@ -23078,11 +23177,13 @@
       <c r="AP33"/>
       <c r="AQ33"/>
       <c r="AR33" s="119" t="s">
-        <v>166</v>
+        <v>1651</v>
       </c>
       <c r="AS33" s="119"/>
       <c r="AT33" s="119"/>
-      <c r="AU33"/>
+      <c r="AU33" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV33"/>
     </row>
     <row r="34" spans="2:48" ht="30" customHeight="1">
@@ -23183,11 +23284,13 @@
       <c r="AP34"/>
       <c r="AQ34"/>
       <c r="AR34" s="119" t="s">
-        <v>166</v>
+        <v>1651</v>
       </c>
       <c r="AS34" s="119"/>
       <c r="AT34" s="119"/>
-      <c r="AU34"/>
+      <c r="AU34" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV34"/>
     </row>
     <row r="35" spans="2:48" ht="30" customHeight="1">
@@ -23285,12 +23388,14 @@
       <c r="AO35"/>
       <c r="AP35"/>
       <c r="AQ35"/>
-      <c r="AR35" s="73" t="s">
-        <v>166</v>
+      <c r="AR35" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS35" s="73"/>
       <c r="AT35" s="73"/>
-      <c r="AU35"/>
+      <c r="AU35" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV35"/>
     </row>
     <row r="36" spans="2:48" ht="30" customHeight="1">
@@ -23388,12 +23493,14 @@
       <c r="AO36"/>
       <c r="AP36"/>
       <c r="AQ36"/>
-      <c r="AR36" s="73" t="s">
-        <v>166</v>
+      <c r="AR36" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS36" s="73"/>
       <c r="AT36" s="73"/>
-      <c r="AU36"/>
+      <c r="AU36" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV36"/>
     </row>
     <row r="37" spans="2:48" ht="30" customHeight="1">
@@ -23493,12 +23600,14 @@
       <c r="AO37"/>
       <c r="AP37"/>
       <c r="AQ37"/>
-      <c r="AR37" s="73" t="s">
-        <v>166</v>
+      <c r="AR37" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS37" s="73"/>
       <c r="AT37" s="73"/>
-      <c r="AU37"/>
+      <c r="AU37" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV37"/>
     </row>
     <row r="38" spans="2:48" ht="30" customHeight="1">
@@ -23598,12 +23707,14 @@
       <c r="AO38"/>
       <c r="AP38"/>
       <c r="AQ38"/>
-      <c r="AR38" s="73" t="s">
-        <v>166</v>
+      <c r="AR38" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS38" s="73"/>
       <c r="AT38" s="73"/>
-      <c r="AU38"/>
+      <c r="AU38" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV38"/>
     </row>
     <row r="39" spans="2:48" ht="30" customHeight="1">
@@ -23702,11 +23813,13 @@
       <c r="AP39"/>
       <c r="AQ39"/>
       <c r="AR39" s="119" t="s">
-        <v>166</v>
+        <v>1651</v>
       </c>
       <c r="AS39" s="119"/>
       <c r="AT39" s="119"/>
-      <c r="AU39"/>
+      <c r="AU39" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV39"/>
     </row>
     <row r="40" spans="2:48" ht="30" customHeight="1">
@@ -23807,11 +23920,13 @@
       <c r="AP40"/>
       <c r="AQ40"/>
       <c r="AR40" s="119" t="s">
-        <v>166</v>
+        <v>1651</v>
       </c>
       <c r="AS40" s="119"/>
       <c r="AT40" s="119"/>
-      <c r="AU40"/>
+      <c r="AU40" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV40"/>
     </row>
     <row r="41" spans="2:48" ht="30" customHeight="1">
@@ -23911,12 +24026,14 @@
       <c r="AO41"/>
       <c r="AP41"/>
       <c r="AQ41"/>
-      <c r="AR41" s="73" t="s">
-        <v>166</v>
+      <c r="AR41" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS41" s="73"/>
       <c r="AT41" s="73"/>
-      <c r="AU41"/>
+      <c r="AU41" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV41"/>
     </row>
     <row r="42" spans="2:48" ht="30" customHeight="1">
@@ -24016,12 +24133,14 @@
       <c r="AO42"/>
       <c r="AP42"/>
       <c r="AQ42"/>
-      <c r="AR42" s="73" t="s">
-        <v>166</v>
+      <c r="AR42" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS42" s="73"/>
       <c r="AT42" s="73"/>
-      <c r="AU42"/>
+      <c r="AU42" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV42"/>
     </row>
     <row r="43" spans="2:48" ht="30" customHeight="1">
@@ -24121,12 +24240,14 @@
       <c r="AO43"/>
       <c r="AP43"/>
       <c r="AQ43"/>
-      <c r="AR43" s="73" t="s">
-        <v>166</v>
+      <c r="AR43" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS43" s="73"/>
       <c r="AT43" s="73"/>
-      <c r="AU43"/>
+      <c r="AU43" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV43"/>
     </row>
     <row r="44" spans="2:48" ht="30" customHeight="1">
@@ -24224,12 +24345,14 @@
       <c r="AO44"/>
       <c r="AP44"/>
       <c r="AQ44"/>
-      <c r="AR44" s="73" t="s">
-        <v>166</v>
+      <c r="AR44" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS44" s="73"/>
       <c r="AT44" s="73"/>
-      <c r="AU44"/>
+      <c r="AU44" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV44"/>
     </row>
     <row r="45" spans="2:48" ht="30" customHeight="1">
@@ -24330,11 +24453,13 @@
       <c r="AP45"/>
       <c r="AQ45"/>
       <c r="AR45" s="119" t="s">
-        <v>166</v>
+        <v>1651</v>
       </c>
       <c r="AS45" s="119"/>
       <c r="AT45" s="119"/>
-      <c r="AU45"/>
+      <c r="AU45" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV45"/>
     </row>
     <row r="46" spans="2:48" ht="30" customHeight="1">
@@ -24429,11 +24554,13 @@
       <c r="AP46"/>
       <c r="AQ46"/>
       <c r="AR46" s="119" t="s">
-        <v>166</v>
+        <v>1651</v>
       </c>
       <c r="AS46" s="119"/>
       <c r="AT46" s="119"/>
-      <c r="AU46"/>
+      <c r="AU46" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV46"/>
     </row>
     <row r="47" spans="2:48" ht="30" customHeight="1">
@@ -24531,12 +24658,14 @@
       <c r="AO47"/>
       <c r="AP47"/>
       <c r="AQ47"/>
-      <c r="AR47" s="73" t="s">
-        <v>166</v>
+      <c r="AR47" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS47" s="73"/>
       <c r="AT47" s="73"/>
-      <c r="AU47"/>
+      <c r="AU47" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV47"/>
     </row>
     <row r="48" spans="2:48" ht="30" customHeight="1">
@@ -24636,12 +24765,14 @@
       <c r="AO48"/>
       <c r="AP48"/>
       <c r="AQ48"/>
-      <c r="AR48" s="29" t="s">
-        <v>1653</v>
+      <c r="AR48" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS48" s="73"/>
       <c r="AT48" s="73"/>
-      <c r="AU48"/>
+      <c r="AU48" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV48"/>
     </row>
     <row r="49" spans="2:48" ht="30" customHeight="1">
@@ -24739,12 +24870,14 @@
       <c r="AO49"/>
       <c r="AP49"/>
       <c r="AQ49"/>
-      <c r="AR49" s="29" t="s">
-        <v>1653</v>
+      <c r="AR49" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS49" s="73"/>
       <c r="AT49" s="73"/>
-      <c r="AU49"/>
+      <c r="AU49" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV49"/>
     </row>
     <row r="50" spans="2:48" ht="30" customHeight="1">
@@ -24836,12 +24969,14 @@
       <c r="AO50"/>
       <c r="AP50"/>
       <c r="AQ50"/>
-      <c r="AR50" s="29" t="s">
-        <v>1653</v>
+      <c r="AR50" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS50" s="73"/>
       <c r="AT50" s="73"/>
-      <c r="AU50"/>
+      <c r="AU50" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV50"/>
     </row>
     <row r="51" spans="2:48" s="55" customFormat="1" ht="30" customHeight="1">
@@ -24914,7 +25049,7 @@
       </c>
       <c r="AK51" s="119"/>
       <c r="AL51" t="s">
-        <v>1572</v>
+        <v>1654</v>
       </c>
       <c r="AM51" s="119" t="s">
         <v>165</v>
@@ -24923,15 +25058,15 @@
       <c r="AO51"/>
       <c r="AP51"/>
       <c r="AQ51"/>
-      <c r="AR51" s="29" t="s">
-        <v>1653</v>
+      <c r="AR51" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS51" s="119" t="s">
-        <v>1585</v>
+        <v>1582</v>
       </c>
       <c r="AT51" s="119"/>
       <c r="AU51" s="132" t="s">
-        <v>1593</v>
+        <v>1655</v>
       </c>
       <c r="AV51" s="119"/>
     </row>
@@ -25021,15 +25156,17 @@
       <c r="AN52"/>
       <c r="AO52"/>
       <c r="AP52" s="119" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="AQ52"/>
-      <c r="AR52" s="29" t="s">
-        <v>1653</v>
+      <c r="AR52" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS52" s="119"/>
       <c r="AT52" s="119"/>
-      <c r="AU52"/>
+      <c r="AU52" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV52"/>
     </row>
     <row r="53" spans="2:48" ht="30" customHeight="1">
@@ -25127,12 +25264,14 @@
       <c r="AO53"/>
       <c r="AP53" s="119"/>
       <c r="AQ53"/>
-      <c r="AR53" s="29" t="s">
-        <v>1653</v>
+      <c r="AR53" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS53" s="73"/>
       <c r="AT53" s="73"/>
-      <c r="AU53" s="132"/>
+      <c r="AU53" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV53"/>
     </row>
     <row r="54" spans="2:48" ht="30" customHeight="1">
@@ -25227,15 +25366,17 @@
       <c r="AN54"/>
       <c r="AO54"/>
       <c r="AP54" s="119" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
       <c r="AQ54"/>
-      <c r="AR54" s="29" t="s">
-        <v>1653</v>
+      <c r="AR54" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS54" s="73"/>
       <c r="AT54" s="73"/>
-      <c r="AU54"/>
+      <c r="AU54" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV54"/>
     </row>
     <row r="55" spans="2:48" ht="30" customHeight="1">
@@ -25333,12 +25474,14 @@
       <c r="AO55"/>
       <c r="AP55" s="119"/>
       <c r="AQ55"/>
-      <c r="AR55" s="29" t="s">
-        <v>1653</v>
+      <c r="AR55" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS55" s="73"/>
       <c r="AT55" s="73"/>
-      <c r="AU55"/>
+      <c r="AU55" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV55"/>
     </row>
     <row r="56" spans="2:48" ht="30" customHeight="1">
@@ -25436,12 +25579,14 @@
       <c r="AO56"/>
       <c r="AP56" s="119"/>
       <c r="AQ56"/>
-      <c r="AR56" s="29" t="s">
-        <v>1653</v>
+      <c r="AR56" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS56" s="73"/>
       <c r="AT56" s="73"/>
-      <c r="AU56"/>
+      <c r="AU56" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV56"/>
     </row>
     <row r="57" spans="2:48" ht="30" customHeight="1">
@@ -25539,12 +25684,14 @@
       <c r="AO57"/>
       <c r="AP57" s="119"/>
       <c r="AQ57"/>
-      <c r="AR57" s="29" t="s">
-        <v>1653</v>
+      <c r="AR57" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS57" s="119"/>
       <c r="AT57" s="119"/>
-      <c r="AU57"/>
+      <c r="AU57" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV57"/>
     </row>
     <row r="58" spans="2:48" ht="30" customHeight="1">
@@ -25642,12 +25789,14 @@
       <c r="AO58"/>
       <c r="AP58" s="119"/>
       <c r="AQ58"/>
-      <c r="AR58" s="29" t="s">
-        <v>1653</v>
+      <c r="AR58" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS58" s="119"/>
       <c r="AT58" s="119"/>
-      <c r="AU58"/>
+      <c r="AU58" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV58"/>
     </row>
     <row r="59" spans="2:48" ht="30" customHeight="1">
@@ -25745,12 +25894,14 @@
       <c r="AO59"/>
       <c r="AP59" s="119"/>
       <c r="AQ59"/>
-      <c r="AR59" s="29" t="s">
-        <v>1653</v>
+      <c r="AR59" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS59" s="73"/>
       <c r="AT59" s="73"/>
-      <c r="AU59"/>
+      <c r="AU59" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV59"/>
     </row>
     <row r="60" spans="2:48" ht="30" customHeight="1">
@@ -25848,12 +25999,14 @@
       <c r="AO60"/>
       <c r="AP60" s="119"/>
       <c r="AQ60"/>
-      <c r="AR60" s="29" t="s">
-        <v>1653</v>
+      <c r="AR60" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS60" s="73"/>
       <c r="AT60" s="73"/>
-      <c r="AU60"/>
+      <c r="AU60" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV60"/>
     </row>
     <row r="61" spans="2:48" ht="30" customHeight="1">
@@ -25953,12 +26106,14 @@
       <c r="AO61"/>
       <c r="AP61" s="119"/>
       <c r="AQ61"/>
-      <c r="AR61" s="29" t="s">
-        <v>1653</v>
+      <c r="AR61" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS61" s="73"/>
       <c r="AT61" s="73"/>
-      <c r="AU61"/>
+      <c r="AU61" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV61"/>
     </row>
     <row r="62" spans="2:48" ht="30" customHeight="1">
@@ -26058,12 +26213,14 @@
       <c r="AO62"/>
       <c r="AP62" s="119"/>
       <c r="AQ62"/>
-      <c r="AR62" s="29" t="s">
-        <v>1653</v>
+      <c r="AR62" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS62" s="73"/>
       <c r="AT62" s="73"/>
-      <c r="AU62"/>
+      <c r="AU62" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV62"/>
     </row>
     <row r="63" spans="2:48" ht="30" customHeight="1">
@@ -26163,12 +26320,14 @@
       <c r="AO63"/>
       <c r="AP63" s="119"/>
       <c r="AQ63"/>
-      <c r="AR63" s="29" t="s">
-        <v>1653</v>
+      <c r="AR63" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS63" s="73"/>
       <c r="AT63" s="73"/>
-      <c r="AU63"/>
+      <c r="AU63" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV63"/>
     </row>
     <row r="64" spans="2:48" ht="30" customHeight="1">
@@ -26264,12 +26423,14 @@
       <c r="AO64"/>
       <c r="AP64" s="119"/>
       <c r="AQ64"/>
-      <c r="AR64" s="29" t="s">
-        <v>1653</v>
+      <c r="AR64" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS64" s="73"/>
       <c r="AT64" s="73"/>
-      <c r="AU64"/>
+      <c r="AU64" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV64"/>
     </row>
     <row r="65" spans="2:48" ht="30" customHeight="1">
@@ -26369,12 +26530,14 @@
       <c r="AO65"/>
       <c r="AP65" s="119"/>
       <c r="AQ65"/>
-      <c r="AR65" s="29" t="s">
-        <v>1653</v>
+      <c r="AR65" s="119" t="s">
+        <v>1651</v>
       </c>
       <c r="AS65" s="73"/>
       <c r="AT65" s="73"/>
-      <c r="AU65"/>
+      <c r="AU65" s="132" t="s">
+        <v>1655</v>
+      </c>
       <c r="AV65"/>
     </row>
   </sheetData>
@@ -26383,15 +26546,74 @@
     <hyperlink ref="AU51" r:id="rId1" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{B537FB82-D68F-844C-B0BC-9141BF70A637}"/>
     <hyperlink ref="AU4" r:id="rId2" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{996E2D0D-DAEB-D84A-AF0D-A265C3B4E575}"/>
     <hyperlink ref="AU8" r:id="rId3" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{B6A2C233-5C21-BE42-96D2-35ABDB919669}"/>
-    <hyperlink ref="AL4" r:id="rId4" xr:uid="{81D8A452-EE1E-45C1-B965-E45AADF56379}"/>
+    <hyperlink ref="AL4" r:id="rId4" display="http://fhir.org/guides/who/anc-cds/StructureDefinition/anc-base-encounter" xr:uid="{81D8A452-EE1E-45C1-B965-E45AADF56379}"/>
     <hyperlink ref="AU3" r:id="rId5" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{78BF62B2-3C71-4EC9-9D78-A4D623B6A233}"/>
+    <hyperlink ref="AU5" r:id="rId6" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{E8A72AB1-29D3-4EFA-89F1-4A85DD9E3E41}"/>
+    <hyperlink ref="AU6" r:id="rId7" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{795F6128-3DBD-4795-B317-72528668B8FD}"/>
+    <hyperlink ref="AU7" r:id="rId8" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{4577D704-1A9B-409B-B05E-1D1006048B5B}"/>
+    <hyperlink ref="AU9" r:id="rId9" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{784ADAC7-D999-46F9-B54C-4958A91B1A06}"/>
+    <hyperlink ref="AU10" r:id="rId10" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{CDB224D4-3DE8-4AF7-988A-BDA08766DD25}"/>
+    <hyperlink ref="AU11" r:id="rId11" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{18B65D88-2708-49BF-8BD8-589EA8B2F73B}"/>
+    <hyperlink ref="AU12" r:id="rId12" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{4BC5E2C2-A36B-4B8C-95E4-F72B3616DEEF}"/>
+    <hyperlink ref="AU13" r:id="rId13" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{7624F451-853C-4393-B081-CA77C5C7D79F}"/>
+    <hyperlink ref="AU14" r:id="rId14" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{A25B5D72-80E2-42D8-8152-C3145BFEB9EA}"/>
+    <hyperlink ref="AU15" r:id="rId15" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{DF3727C7-6833-406C-A362-6B3DF3270475}"/>
+    <hyperlink ref="AU16" r:id="rId16" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{4BADD552-3906-4867-849C-D2A35DF1AE37}"/>
+    <hyperlink ref="AU17" r:id="rId17" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{87981801-7F61-4164-90A7-7DB995AEE642}"/>
+    <hyperlink ref="AU18" r:id="rId18" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{CB5844D6-278E-42C7-BFD8-468A65AD20C9}"/>
+    <hyperlink ref="AU19" r:id="rId19" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{E63D1834-D4F3-4078-A148-55A06BF4FEF5}"/>
+    <hyperlink ref="AU20" r:id="rId20" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{DE4B0099-33DB-4E65-B231-C76262AC887D}"/>
+    <hyperlink ref="AU21" r:id="rId21" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{BC77EA96-1382-42C5-BA54-A1E9923A5B1C}"/>
+    <hyperlink ref="AU22" r:id="rId22" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{D7DDAF70-FD98-4445-9843-8D6F8C7C8208}"/>
+    <hyperlink ref="AU23" r:id="rId23" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{39A116D9-99AD-43EF-81F9-69E0CA0FA4E4}"/>
+    <hyperlink ref="AU24" r:id="rId24" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{1F757472-CB86-4895-9567-5539FDAD4A1A}"/>
+    <hyperlink ref="AU25" r:id="rId25" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{A6B908AA-B74A-47B2-B332-DABA5FD516A4}"/>
+    <hyperlink ref="AU26" r:id="rId26" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{D7BDA6A2-FDD0-4D8F-A3C6-41CDC0F8E33B}"/>
+    <hyperlink ref="AU27" r:id="rId27" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{9A3E8DDB-6D77-4C52-B8C9-AE4F6129D07B}"/>
+    <hyperlink ref="AU28" r:id="rId28" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{44FBE4AB-360C-4A74-A416-6FC20F93D072}"/>
+    <hyperlink ref="AU29" r:id="rId29" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{EB1AE14D-868C-4FCF-B6FF-6988A4734D64}"/>
+    <hyperlink ref="AU30" r:id="rId30" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{AAC72F51-80F5-4F2A-BDFC-39A5C3BC781D}"/>
+    <hyperlink ref="AU31" r:id="rId31" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{538873DC-0EBD-45A9-B28D-751DEA530344}"/>
+    <hyperlink ref="AU32" r:id="rId32" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{21502DAD-3382-489B-903B-8F47E8A534FD}"/>
+    <hyperlink ref="AU33" r:id="rId33" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{95AEF298-0345-4C64-86AB-BCB45A768FA2}"/>
+    <hyperlink ref="AU34" r:id="rId34" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{24F8D838-7CB4-41BB-8F19-852A7FCDF826}"/>
+    <hyperlink ref="AU35" r:id="rId35" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{8264461A-1B53-421B-B7E1-3F2655B690F1}"/>
+    <hyperlink ref="AU36" r:id="rId36" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{15F7ABBD-425E-4E95-83E1-6ABDF7D8561C}"/>
+    <hyperlink ref="AU37" r:id="rId37" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{47AC6B1D-06EA-4B80-8D2B-C624AA6E1579}"/>
+    <hyperlink ref="AU38" r:id="rId38" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{8AFA5BA0-5A61-4200-9107-2C29E5425A30}"/>
+    <hyperlink ref="AU39" r:id="rId39" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{06340ED0-B6C6-4395-AFB4-DC29F31A8AA8}"/>
+    <hyperlink ref="AU40" r:id="rId40" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{3AF017C7-F5CF-4E3E-AF3E-9E6FBC1ACB67}"/>
+    <hyperlink ref="AU41" r:id="rId41" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{1C4E4E76-4790-41D6-9FDE-F1A26AC8E431}"/>
+    <hyperlink ref="AU42" r:id="rId42" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{AA1854E1-CDDA-48F2-8F4C-B34E57E02BBC}"/>
+    <hyperlink ref="AU43" r:id="rId43" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{D1C0E904-C088-4A19-885B-32A103D7780D}"/>
+    <hyperlink ref="AU44" r:id="rId44" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{C18AE5FB-DC62-4D1E-840A-4C84E3DA3CB3}"/>
+    <hyperlink ref="AU45" r:id="rId45" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{8CE79EFE-C843-4C72-8846-575786645E1F}"/>
+    <hyperlink ref="AU46" r:id="rId46" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{8E406BE0-6289-4942-8008-89EBBFC9052D}"/>
+    <hyperlink ref="AU47" r:id="rId47" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{D6CE3334-BD33-4911-AD0C-64C756D94ABA}"/>
+    <hyperlink ref="AU48" r:id="rId48" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{464C9B66-2B61-4CF8-88A0-483CFE680639}"/>
+    <hyperlink ref="AU49" r:id="rId49" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{8417946A-2038-4E15-B259-F34F46AEACE4}"/>
+    <hyperlink ref="AU50" r:id="rId50" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{5020ADFB-EC03-4067-8282-2B9E72582A17}"/>
+    <hyperlink ref="AU52" r:id="rId51" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{35CA832A-2076-43AE-A479-E8E839BB10B5}"/>
+    <hyperlink ref="AU53" r:id="rId52" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{93618D6D-F860-4810-828A-CE7E8EE32C31}"/>
+    <hyperlink ref="AU54" r:id="rId53" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{27F16097-BB98-43E8-8237-D2C4416AEE88}"/>
+    <hyperlink ref="AU55" r:id="rId54" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{C292022D-87FA-4422-9579-18BDF103E319}"/>
+    <hyperlink ref="AU56" r:id="rId55" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{863271D9-FE8D-43B3-97B5-6BE7DC7A9D25}"/>
+    <hyperlink ref="AU57" r:id="rId56" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{98D2940C-4FF0-47AC-93E2-6E01DBC23166}"/>
+    <hyperlink ref="AU58" r:id="rId57" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{8C680B53-6280-491E-990D-46CBE96B817B}"/>
+    <hyperlink ref="AU59" r:id="rId58" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{D9010E80-9281-4B99-A06F-69BC9571A6CA}"/>
+    <hyperlink ref="AU60" r:id="rId59" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{C8D4BFF0-3650-40F8-BD84-5BEE2269EDC8}"/>
+    <hyperlink ref="AU61" r:id="rId60" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{33325893-F914-4917-AEF7-4FB4A2D9C4FA}"/>
+    <hyperlink ref="AU62" r:id="rId61" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{E5C24C7B-99BE-4588-87BE-B3DE153EAD83}"/>
+    <hyperlink ref="AU63" r:id="rId62" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{11553846-D0CA-4F08-94F3-FFB5A2114238}"/>
+    <hyperlink ref="AU64" r:id="rId63" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{1D1F2CA6-9F18-476B-B448-A64465883B65}"/>
+    <hyperlink ref="AU65" r:id="rId64" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{13DD22BD-DEFB-481B-9B7E-D5880689B584}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId6"/>
-  <drawing r:id="rId7"/>
+  <pageSetup orientation="landscape" r:id="rId65"/>
+  <drawing r:id="rId66"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C8279A1B-21CF-4FA5-BE58-FF44EC2024A5}">
           <x14:formula1>
             <xm:f>'READ ME'!$C$33:$C$36</xm:f>
@@ -26427,10 +26649,10 @@
   <dimension ref="A1:AS20"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="AF3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="AD3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="AN4" sqref="AN4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="13.15"/>
@@ -26886,7 +27108,7 @@
         <v>74</v>
       </c>
       <c r="I7" s="21" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
       <c r="J7" s="21" t="s">
         <v>1110</v>
@@ -27083,7 +27305,7 @@
         <v>74</v>
       </c>
       <c r="I10" s="21" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
       <c r="J10" s="21"/>
       <c r="K10" s="21" t="s">
@@ -27776,11 +27998,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D470B58E-E520-4467-BD8B-F78DD56D2F42}">
   <dimension ref="A1:AV61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="3" topLeftCell="AL19" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="6" ySplit="3" topLeftCell="AO20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AQ25" sqref="AQ25"/>
+      <selection pane="bottomRight" activeCell="AR25" sqref="AR25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="13.15"/>
@@ -28073,7 +28295,7 @@
         <v>290</v>
       </c>
       <c r="AK3" s="60" t="s">
-        <v>1572</v>
+        <v>1654</v>
       </c>
       <c r="AL3" s="60" t="s">
         <v>165</v>
@@ -28081,11 +28303,11 @@
       <c r="AP3" s="60" t="s">
         <v>1085</v>
       </c>
-      <c r="AQ3" s="60" t="s">
-        <v>1653</v>
+      <c r="AQ3" s="29" t="s">
+        <v>1651</v>
       </c>
       <c r="AR3" s="142" t="s">
-        <v>1593</v>
+        <v>1655</v>
       </c>
       <c r="AS3" s="67"/>
       <c r="AT3" s="67"/>
@@ -28175,8 +28397,11 @@
       <c r="AL4" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="AQ4" s="60" t="s">
-        <v>1653</v>
+      <c r="AQ4" s="29" t="s">
+        <v>1651</v>
+      </c>
+      <c r="AR4" s="142" t="s">
+        <v>1655</v>
       </c>
     </row>
     <row r="5" spans="1:48" ht="30" customHeight="1">
@@ -28264,8 +28489,11 @@
       <c r="AL5" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="AQ5" s="60" t="s">
-        <v>1653</v>
+      <c r="AQ5" s="29" t="s">
+        <v>1651</v>
+      </c>
+      <c r="AR5" s="142" t="s">
+        <v>1655</v>
       </c>
     </row>
     <row r="6" spans="1:48" ht="30" customHeight="1">
@@ -28353,8 +28581,11 @@
       <c r="AL6" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="AQ6" s="60" t="s">
-        <v>1653</v>
+      <c r="AQ6" s="29" t="s">
+        <v>1651</v>
+      </c>
+      <c r="AR6" s="142" t="s">
+        <v>1655</v>
       </c>
     </row>
     <row r="7" spans="1:48" ht="30" customHeight="1">
@@ -28442,8 +28673,11 @@
       <c r="AL7" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="AQ7" s="60" t="s">
-        <v>1653</v>
+      <c r="AQ7" s="29" t="s">
+        <v>1651</v>
+      </c>
+      <c r="AR7" s="142" t="s">
+        <v>1655</v>
       </c>
     </row>
     <row r="8" spans="1:48" ht="30" customHeight="1">
@@ -28531,8 +28765,11 @@
       <c r="AL8" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="AQ8" s="60" t="s">
-        <v>1653</v>
+      <c r="AQ8" s="29" t="s">
+        <v>1651</v>
+      </c>
+      <c r="AR8" s="142" t="s">
+        <v>1655</v>
       </c>
     </row>
     <row r="9" spans="1:48" ht="30" customHeight="1">
@@ -28611,8 +28848,11 @@
       <c r="AL9" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="AQ9" s="60" t="s">
-        <v>1653</v>
+      <c r="AQ9" s="29" t="s">
+        <v>1651</v>
+      </c>
+      <c r="AR9" s="142" t="s">
+        <v>1655</v>
       </c>
     </row>
     <row r="10" spans="1:48" ht="30" customHeight="1">
@@ -28691,8 +28931,11 @@
       <c r="AL10" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="AQ10" s="60" t="s">
-        <v>1653</v>
+      <c r="AQ10" s="29" t="s">
+        <v>1651</v>
+      </c>
+      <c r="AR10" s="142" t="s">
+        <v>1655</v>
       </c>
     </row>
     <row r="11" spans="1:48" ht="30" customHeight="1">
@@ -28771,8 +29014,11 @@
       <c r="AL11" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="AQ11" s="60" t="s">
-        <v>1653</v>
+      <c r="AQ11" s="29" t="s">
+        <v>1651</v>
+      </c>
+      <c r="AR11" s="142" t="s">
+        <v>1655</v>
       </c>
     </row>
     <row r="12" spans="1:48" ht="30" customHeight="1">
@@ -28845,8 +29091,11 @@
       <c r="AL12" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="AQ12" s="60" t="s">
-        <v>1653</v>
+      <c r="AQ12" s="29" t="s">
+        <v>1651</v>
+      </c>
+      <c r="AR12" s="142" t="s">
+        <v>1655</v>
       </c>
     </row>
     <row r="13" spans="1:48" ht="30" customHeight="1">
@@ -28926,8 +29175,11 @@
       <c r="AL13" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="AQ13" s="60" t="s">
-        <v>1653</v>
+      <c r="AQ13" s="29" t="s">
+        <v>1651</v>
+      </c>
+      <c r="AR13" s="142" t="s">
+        <v>1655</v>
       </c>
     </row>
     <row r="14" spans="1:48" ht="30" customHeight="1">
@@ -29010,16 +29262,16 @@
         <v>164</v>
       </c>
       <c r="AK14" s="29" t="s">
-        <v>1572</v>
+        <v>1654</v>
       </c>
       <c r="AL14" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="AQ14" s="60" t="s">
-        <v>1653</v>
+      <c r="AQ14" s="29" t="s">
+        <v>1651</v>
       </c>
       <c r="AR14" s="142" t="s">
-        <v>1593</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="15" spans="1:48" s="60" customFormat="1" ht="30" customHeight="1">
@@ -29097,11 +29349,11 @@
       <c r="AP15" s="60" t="s">
         <v>1085</v>
       </c>
-      <c r="AQ15" s="60" t="s">
-        <v>1653</v>
+      <c r="AQ15" s="29" t="s">
+        <v>1651</v>
       </c>
       <c r="AR15" s="142" t="s">
-        <v>1593</v>
+        <v>1655</v>
       </c>
       <c r="AS15" s="67"/>
       <c r="AT15" s="67"/>
@@ -29197,8 +29449,11 @@
       <c r="AL16" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="AQ16" s="60" t="s">
-        <v>1653</v>
+      <c r="AQ16" s="29" t="s">
+        <v>1651</v>
+      </c>
+      <c r="AR16" s="142" t="s">
+        <v>1655</v>
       </c>
     </row>
     <row r="17" spans="1:44" ht="30" customHeight="1">
@@ -29286,8 +29541,11 @@
       <c r="AL17" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="AQ17" s="60" t="s">
-        <v>1653</v>
+      <c r="AQ17" s="29" t="s">
+        <v>1651</v>
+      </c>
+      <c r="AR17" s="142" t="s">
+        <v>1655</v>
       </c>
     </row>
     <row r="18" spans="1:44" ht="30" customHeight="1">
@@ -29375,8 +29633,11 @@
       <c r="AL18" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="AQ18" s="60" t="s">
-        <v>1653</v>
+      <c r="AQ18" s="29" t="s">
+        <v>1651</v>
+      </c>
+      <c r="AR18" s="142" t="s">
+        <v>1655</v>
       </c>
     </row>
     <row r="19" spans="1:44" ht="30" customHeight="1">
@@ -29461,16 +29722,16 @@
         <v>264</v>
       </c>
       <c r="AK19" s="29" t="s">
-        <v>1572</v>
+        <v>1654</v>
       </c>
       <c r="AL19" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="AQ19" s="60" t="s">
-        <v>1653</v>
+      <c r="AQ19" s="29" t="s">
+        <v>1651</v>
       </c>
       <c r="AR19" s="142" t="s">
-        <v>1593</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="20" spans="1:44" s="60" customFormat="1" ht="30" customHeight="1">
@@ -29540,16 +29801,16 @@
         <v>290</v>
       </c>
       <c r="AK20" s="60" t="s">
-        <v>1572</v>
+        <v>1654</v>
       </c>
       <c r="AL20" s="60" t="s">
         <v>165</v>
       </c>
-      <c r="AQ20" s="60" t="s">
-        <v>1653</v>
+      <c r="AQ20" s="29" t="s">
+        <v>1651</v>
       </c>
       <c r="AR20" s="142" t="s">
-        <v>1593</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="21" spans="1:44" ht="30" customHeight="1">
@@ -29640,8 +29901,11 @@
       <c r="AL21" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="AQ21" s="60" t="s">
-        <v>1653</v>
+      <c r="AQ21" s="29" t="s">
+        <v>1651</v>
+      </c>
+      <c r="AR21" s="142" t="s">
+        <v>1655</v>
       </c>
     </row>
     <row r="22" spans="1:44" ht="30" customHeight="1">
@@ -29732,8 +29996,11 @@
       <c r="AL22" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="AQ22" s="60" t="s">
-        <v>1653</v>
+      <c r="AQ22" s="29" t="s">
+        <v>1651</v>
+      </c>
+      <c r="AR22" s="142" t="s">
+        <v>1655</v>
       </c>
     </row>
     <row r="23" spans="1:44" ht="30" customHeight="1">
@@ -29815,8 +30082,11 @@
       <c r="AL23" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="AQ23" s="60" t="s">
-        <v>1653</v>
+      <c r="AQ23" s="29" t="s">
+        <v>1651</v>
+      </c>
+      <c r="AR23" s="142" t="s">
+        <v>1655</v>
       </c>
     </row>
     <row r="24" spans="1:44" ht="30" customHeight="1">
@@ -29907,8 +30177,11 @@
       <c r="AL24" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="AQ24" s="60" t="s">
-        <v>1653</v>
+      <c r="AQ24" s="29" t="s">
+        <v>1651</v>
+      </c>
+      <c r="AR24" s="142" t="s">
+        <v>1655</v>
       </c>
     </row>
     <row r="25" spans="1:44" ht="30" customHeight="1">
@@ -30000,16 +30273,16 @@
         <v>58</v>
       </c>
       <c r="AK25" s="29" t="s">
-        <v>1572</v>
+        <v>1654</v>
       </c>
       <c r="AL25" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="AQ25" s="60" t="s">
-        <v>1653</v>
+      <c r="AQ25" s="29" t="s">
+        <v>1651</v>
       </c>
       <c r="AR25" s="142" t="s">
-        <v>1593</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="26" spans="1:44" ht="30" customHeight="1">
@@ -30434,7 +30707,7 @@
         <v>264</v>
       </c>
       <c r="AK35" s="29" t="s">
-        <v>1572</v>
+        <v>1654</v>
       </c>
       <c r="AL35" s="29" t="s">
         <v>165</v>
@@ -30510,7 +30783,7 @@
         <v>290</v>
       </c>
       <c r="AK36" s="60" t="s">
-        <v>1572</v>
+        <v>1654</v>
       </c>
       <c r="AL36" s="60" t="s">
         <v>165</v>
@@ -30522,7 +30795,7 @@
         <v>166</v>
       </c>
       <c r="AR36" s="142" t="s">
-        <v>1593</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="37" spans="1:44" ht="30" customHeight="1">
@@ -31589,7 +31862,7 @@
         <v>164</v>
       </c>
       <c r="AK49" s="29" t="s">
-        <v>1572</v>
+        <v>1654</v>
       </c>
       <c r="AL49" s="29" t="s">
         <v>165</v>
@@ -31675,7 +31948,7 @@
         <v>164</v>
       </c>
       <c r="AK50" s="29" t="s">
-        <v>1572</v>
+        <v>1654</v>
       </c>
       <c r="AL50" s="29" t="s">
         <v>165</v>
@@ -31751,7 +32024,7 @@
         <v>290</v>
       </c>
       <c r="AK51" s="60" t="s">
-        <v>1572</v>
+        <v>1654</v>
       </c>
       <c r="AL51" s="60" t="s">
         <v>165</v>
@@ -31763,7 +32036,7 @@
         <v>166</v>
       </c>
       <c r="AR51" s="142" t="s">
-        <v>1593</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="52" spans="1:44" ht="30" customHeight="1">
@@ -32639,12 +32912,29 @@
     <hyperlink ref="AR25" r:id="rId6" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{076EB715-3DF7-42DD-99E5-6BA487313CD6}"/>
     <hyperlink ref="AR36" r:id="rId7" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{A561F7DD-79AA-4904-A971-9773848CFBDA}"/>
     <hyperlink ref="AR51" r:id="rId8" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{408F63F5-BACB-4653-B6DF-E7B9F03E9756}"/>
+    <hyperlink ref="AR4" r:id="rId9" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{B6E7A9BF-C4C9-40BE-B493-D6600F541311}"/>
+    <hyperlink ref="AR5" r:id="rId10" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{F2C5D4AA-AC89-4E3A-B86F-04EE6C260BCD}"/>
+    <hyperlink ref="AR6" r:id="rId11" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{392B7E7D-DEDD-487A-8524-98528B2418B3}"/>
+    <hyperlink ref="AR7" r:id="rId12" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{215E2B41-ACC8-447A-88A7-F5D1D2AAF7C7}"/>
+    <hyperlink ref="AR8" r:id="rId13" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{6E3EC43C-4921-48B4-ABF8-75CB12DAB405}"/>
+    <hyperlink ref="AR9" r:id="rId14" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{54BAF09D-176C-4078-8EA5-724004F57E1B}"/>
+    <hyperlink ref="AR10" r:id="rId15" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{C7470352-DCCD-4E5C-A368-22E28D1B1016}"/>
+    <hyperlink ref="AR11" r:id="rId16" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{C7652DA4-2B4A-4C27-85C1-1B267F5E741B}"/>
+    <hyperlink ref="AR12" r:id="rId17" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{1129429C-4710-44FF-97F4-B8E0DD48772C}"/>
+    <hyperlink ref="AR13" r:id="rId18" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{AD94A267-1F72-42ED-B94F-164B29F8C677}"/>
+    <hyperlink ref="AR16" r:id="rId19" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{87704415-B69A-492E-86CE-2ECCADF3C3B1}"/>
+    <hyperlink ref="AR17" r:id="rId20" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{92872522-414A-4388-8A12-FE194A06483E}"/>
+    <hyperlink ref="AR18" r:id="rId21" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{F629A805-8584-4411-9C45-D8AC787E6D7B}"/>
+    <hyperlink ref="AR21" r:id="rId22" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{AC0FB6E5-54DA-46FA-9B29-FA7FA86AA011}"/>
+    <hyperlink ref="AR22" r:id="rId23" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{BA4E12AD-05B3-4B98-85E0-4599DDBBAE2F}"/>
+    <hyperlink ref="AR23" r:id="rId24" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{CAC9BC60-14FC-41AD-B321-DE8F812D296E}"/>
+    <hyperlink ref="AR24" r:id="rId25" display="http://fhir.org/guides/who/anc-cds/CodeSystem/anc-custom" xr:uid="{3129E755-3DAB-4DA2-868C-8D2615312401}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId26"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FEB6BE94-3176-4604-B47B-6D6BE1078447}">
           <x14:formula1>
             <xm:f>'READ ME'!$C$33:$C$36</xm:f>

</xml_diff>

<commit_message>
Added Danger Signs PlanDefinition
</commit_message>
<xml_diff>
--- a/input/l2/WHO-ANC-mini.xlsx
+++ b/input/l2/WHO-ANC-mini.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryn\Documents\Src\WHO\smart-anc-mini\input\l2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D77A5F-1DE8-4FC9-9A0F-83F9433B65F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32CB827F-5F79-4920-B1FF-DFBC7322EF37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="1238" windowWidth="21600" windowHeight="11512" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4011" yWindow="4011" windowWidth="24686" windowHeight="13260" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="17" r:id="rId1"/>
@@ -16295,16 +16295,16 @@
       <selection activeCell="B10" sqref="B10:J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.45"/>
   <cols>
-    <col min="1" max="1" width="3.73046875" customWidth="1"/>
-    <col min="2" max="2" width="32.265625" customWidth="1"/>
-    <col min="5" max="5" width="16.73046875" customWidth="1"/>
-    <col min="7" max="7" width="8.3984375" customWidth="1"/>
-    <col min="10" max="10" width="25.1328125" customWidth="1"/>
+    <col min="1" max="1" width="3.69140625" customWidth="1"/>
+    <col min="2" max="2" width="32.3046875" customWidth="1"/>
+    <col min="5" max="5" width="16.69140625" customWidth="1"/>
+    <col min="7" max="7" width="8.3828125" customWidth="1"/>
+    <col min="10" max="10" width="25.15234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" s="90" customFormat="1" ht="14.25">
+    <row r="2" spans="2:11" s="90" customFormat="1" ht="14.6">
       <c r="B2" s="155"/>
       <c r="C2" s="155"/>
       <c r="D2" s="155"/>
@@ -16315,7 +16315,7 @@
       <c r="I2" s="155"/>
       <c r="J2" s="155"/>
     </row>
-    <row r="3" spans="2:11" s="90" customFormat="1" ht="14.25">
+    <row r="3" spans="2:11" s="90" customFormat="1" ht="14.6">
       <c r="B3" s="155"/>
       <c r="C3" s="155"/>
       <c r="D3" s="155"/>
@@ -16326,7 +16326,7 @@
       <c r="I3" s="155"/>
       <c r="J3" s="155"/>
     </row>
-    <row r="4" spans="2:11" s="90" customFormat="1" ht="14.25">
+    <row r="4" spans="2:11" s="90" customFormat="1" ht="14.6">
       <c r="B4" s="155"/>
       <c r="C4" s="155"/>
       <c r="D4" s="155"/>
@@ -16337,7 +16337,7 @@
       <c r="I4" s="155"/>
       <c r="J4" s="155"/>
     </row>
-    <row r="5" spans="2:11" s="90" customFormat="1" ht="14.25">
+    <row r="5" spans="2:11" s="90" customFormat="1" ht="14.6">
       <c r="B5" s="155"/>
       <c r="C5" s="155"/>
       <c r="D5" s="155"/>
@@ -16348,7 +16348,7 @@
       <c r="I5" s="155"/>
       <c r="J5" s="155"/>
     </row>
-    <row r="6" spans="2:11" s="90" customFormat="1" ht="14.25">
+    <row r="6" spans="2:11" s="90" customFormat="1" ht="14.6">
       <c r="B6" s="155"/>
       <c r="C6" s="155"/>
       <c r="D6" s="155"/>
@@ -16359,7 +16359,7 @@
       <c r="I6" s="155"/>
       <c r="J6" s="155"/>
     </row>
-    <row r="7" spans="2:11" s="90" customFormat="1" ht="14.25">
+    <row r="7" spans="2:11" s="90" customFormat="1" ht="14.6">
       <c r="B7" s="155"/>
       <c r="C7" s="155"/>
       <c r="D7" s="155"/>
@@ -16370,7 +16370,7 @@
       <c r="I7" s="155"/>
       <c r="J7" s="155"/>
     </row>
-    <row r="8" spans="2:11" s="90" customFormat="1" ht="14.25">
+    <row r="8" spans="2:11" s="90" customFormat="1" ht="14.6">
       <c r="B8" s="155"/>
       <c r="C8" s="155"/>
       <c r="D8" s="155"/>
@@ -16381,7 +16381,7 @@
       <c r="I8" s="155"/>
       <c r="J8" s="155"/>
     </row>
-    <row r="9" spans="2:11" s="90" customFormat="1" ht="14.25">
+    <row r="9" spans="2:11" s="90" customFormat="1" ht="14.6">
       <c r="B9" s="155"/>
       <c r="C9" s="155"/>
       <c r="D9" s="155"/>
@@ -16405,8 +16405,8 @@
       <c r="I10" s="157"/>
       <c r="J10" s="157"/>
     </row>
-    <row r="11" spans="2:11" ht="13.15" thickBot="1"/>
-    <row r="12" spans="2:11" s="90" customFormat="1" ht="15" thickTop="1" thickBot="1">
+    <row r="11" spans="2:11" ht="12.9" thickBot="1"/>
+    <row r="12" spans="2:11" s="90" customFormat="1" ht="15.45" thickTop="1" thickBot="1">
       <c r="B12" s="133" t="s">
         <v>0</v>
       </c>
@@ -16421,7 +16421,7 @@
       <c r="I12" s="156"/>
       <c r="J12" s="156"/>
     </row>
-    <row r="13" spans="2:11" s="90" customFormat="1" ht="15" thickTop="1" thickBot="1">
+    <row r="13" spans="2:11" s="90" customFormat="1" ht="15.45" thickTop="1" thickBot="1">
       <c r="B13" s="92" t="s">
         <v>2</v>
       </c>
@@ -16436,7 +16436,7 @@
       <c r="I13" s="153"/>
       <c r="J13" s="154"/>
     </row>
-    <row r="14" spans="2:11" s="90" customFormat="1" ht="15" thickTop="1" thickBot="1">
+    <row r="14" spans="2:11" s="90" customFormat="1" ht="15.45" thickTop="1" thickBot="1">
       <c r="B14" s="94" t="s">
         <v>4</v>
       </c>
@@ -16451,7 +16451,7 @@
       <c r="I14" s="153"/>
       <c r="J14" s="154"/>
     </row>
-    <row r="15" spans="2:11" s="90" customFormat="1" ht="15" thickTop="1" thickBot="1">
+    <row r="15" spans="2:11" s="90" customFormat="1" ht="15.45" thickTop="1" thickBot="1">
       <c r="B15" s="94" t="s">
         <v>6</v>
       </c>
@@ -16466,7 +16466,7 @@
       <c r="I15" s="153"/>
       <c r="J15" s="154"/>
     </row>
-    <row r="16" spans="2:11" s="90" customFormat="1" ht="15" thickTop="1" thickBot="1">
+    <row r="16" spans="2:11" s="90" customFormat="1" ht="15.45" thickTop="1" thickBot="1">
       <c r="B16" s="99" t="s">
         <v>8</v>
       </c>
@@ -16482,7 +16482,7 @@
       <c r="J16" s="151"/>
       <c r="K16" s="82"/>
     </row>
-    <row r="17" spans="1:11" s="90" customFormat="1" ht="15" thickTop="1" thickBot="1">
+    <row r="17" spans="1:11" s="90" customFormat="1" ht="15.45" thickTop="1" thickBot="1">
       <c r="B17" s="99" t="s">
         <v>10</v>
       </c>
@@ -16498,7 +16498,7 @@
       <c r="J17" s="151"/>
       <c r="K17" s="82"/>
     </row>
-    <row r="18" spans="1:11" s="90" customFormat="1" ht="15" thickTop="1" thickBot="1">
+    <row r="18" spans="1:11" s="90" customFormat="1" ht="15.45" thickTop="1" thickBot="1">
       <c r="B18" s="99" t="s">
         <v>12</v>
       </c>
@@ -16514,7 +16514,7 @@
       <c r="J18" s="151"/>
       <c r="K18" s="82"/>
     </row>
-    <row r="19" spans="1:11" s="90" customFormat="1" ht="15" thickTop="1" thickBot="1">
+    <row r="19" spans="1:11" s="90" customFormat="1" ht="15.45" thickTop="1" thickBot="1">
       <c r="B19" s="99" t="s">
         <v>14</v>
       </c>
@@ -16530,7 +16530,7 @@
       <c r="J19" s="151"/>
       <c r="K19" s="82"/>
     </row>
-    <row r="20" spans="1:11" s="90" customFormat="1" ht="15" thickTop="1" thickBot="1">
+    <row r="20" spans="1:11" s="90" customFormat="1" ht="15.45" thickTop="1" thickBot="1">
       <c r="B20" s="99" t="s">
         <v>16</v>
       </c>
@@ -16546,7 +16546,7 @@
       <c r="J20" s="151"/>
       <c r="K20" s="82"/>
     </row>
-    <row r="21" spans="1:11" s="90" customFormat="1" ht="15" thickTop="1" thickBot="1">
+    <row r="21" spans="1:11" s="90" customFormat="1" ht="15.45" thickTop="1" thickBot="1">
       <c r="A21" s="93"/>
       <c r="B21" s="94" t="s">
         <v>18</v>
@@ -16577,7 +16577,7 @@
       <c r="I22" s="150"/>
       <c r="J22" s="151"/>
     </row>
-    <row r="23" spans="1:11" ht="13.15" thickTop="1"/>
+    <row r="23" spans="1:11" ht="12.9" thickTop="1"/>
     <row r="24" spans="1:11" ht="27" customHeight="1">
       <c r="B24" s="147" t="s">
         <v>22</v>
@@ -16632,13 +16632,13 @@
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="1" width="3.1328125" style="90" customWidth="1"/>
-    <col min="2" max="2" width="46.73046875" style="90" customWidth="1"/>
-    <col min="3" max="3" width="28.265625" style="90" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.1328125" style="90" customWidth="1"/>
-    <col min="5" max="16384" width="9.1328125" style="90"/>
+    <col min="1" max="1" width="3.15234375" style="90" customWidth="1"/>
+    <col min="2" max="2" width="46.69140625" style="90" customWidth="1"/>
+    <col min="3" max="3" width="28.3046875" style="90" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.15234375" style="90" customWidth="1"/>
+    <col min="5" max="16384" width="9.15234375" style="90"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10">
@@ -16670,7 +16670,7 @@
       <c r="G3" s="98"/>
       <c r="J3" s="82"/>
     </row>
-    <row r="4" spans="2:10" ht="28.9" thickBot="1">
+    <row r="4" spans="2:10" ht="29.6" thickBot="1">
       <c r="B4" s="100" t="s">
         <v>25</v>
       </c>
@@ -16687,7 +16687,7 @@
       <c r="I4" s="82"/>
       <c r="J4" s="82"/>
     </row>
-    <row r="5" spans="2:10" ht="85.9" thickBot="1">
+    <row r="5" spans="2:10" ht="87.9" thickBot="1">
       <c r="B5" s="136" t="s">
         <v>28</v>
       </c>
@@ -16728,7 +16728,7 @@
       <c r="E9" s="82"/>
       <c r="F9" s="82"/>
     </row>
-    <row r="10" spans="2:10" ht="128.65" thickBot="1">
+    <row r="10" spans="2:10" ht="146.15" thickBot="1">
       <c r="B10" s="80" t="s">
         <v>32</v>
       </c>
@@ -16739,7 +16739,7 @@
       <c r="E10" s="82"/>
       <c r="F10" s="82"/>
     </row>
-    <row r="11" spans="2:10" ht="57">
+    <row r="11" spans="2:10" ht="58.3">
       <c r="B11" s="80" t="s">
         <v>34</v>
       </c>
@@ -16766,7 +16766,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="28.5">
+    <row r="14" spans="2:10" ht="29.15">
       <c r="B14" s="160"/>
       <c r="C14" s="135" t="s">
         <v>40</v>
@@ -16775,7 +16775,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="43.15" thickBot="1">
+    <row r="15" spans="2:10" ht="44.15" thickBot="1">
       <c r="B15" s="161"/>
       <c r="C15" s="83" t="s">
         <v>42</v>
@@ -16811,7 +16811,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="28.5">
+    <row r="19" spans="2:4" ht="29.15">
       <c r="B19" s="160"/>
       <c r="C19" s="135" t="s">
         <v>50</v>
@@ -16820,7 +16820,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="28.5">
+    <row r="20" spans="2:4" ht="29.15">
       <c r="B20" s="160"/>
       <c r="C20" s="135" t="s">
         <v>52</v>
@@ -16829,7 +16829,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="28.5">
+    <row r="21" spans="2:4" ht="29.15">
       <c r="B21" s="160"/>
       <c r="C21" s="135" t="s">
         <v>54</v>
@@ -16861,7 +16861,7 @@
       <c r="C24" s="160"/>
       <c r="D24" s="165"/>
     </row>
-    <row r="25" spans="2:4" ht="57">
+    <row r="25" spans="2:4" ht="58.3">
       <c r="B25" s="160"/>
       <c r="C25" s="135" t="s">
         <v>60</v>
@@ -16870,7 +16870,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="2:4" ht="28.5">
+    <row r="26" spans="2:4" ht="29.15">
       <c r="B26" s="160"/>
       <c r="C26" s="135" t="s">
         <v>62</v>
@@ -16879,7 +16879,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="2:4" ht="71.25">
+    <row r="27" spans="2:4" ht="72.900000000000006">
       <c r="B27" s="160"/>
       <c r="C27" s="135" t="s">
         <v>64</v>
@@ -16888,7 +16888,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="2:4" ht="57">
+    <row r="28" spans="2:4" ht="72.900000000000006">
       <c r="B28" s="160"/>
       <c r="C28" s="135" t="s">
         <v>66</v>
@@ -16909,7 +16909,7 @@
       <c r="C30" s="168"/>
       <c r="D30" s="169"/>
     </row>
-    <row r="31" spans="2:4" ht="57.4" thickBot="1">
+    <row r="31" spans="2:4" ht="58.75" thickBot="1">
       <c r="B31" s="80" t="s">
         <v>69</v>
       </c>
@@ -16918,7 +16918,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="2:4" ht="171.4" thickBot="1">
+    <row r="32" spans="2:4" ht="175.3" thickBot="1">
       <c r="B32" s="80" t="s">
         <v>71</v>
       </c>
@@ -16927,7 +16927,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="2:4" ht="42.75">
+    <row r="33" spans="2:4" ht="43.75">
       <c r="B33" s="159" t="s">
         <v>73</v>
       </c>
@@ -16938,7 +16938,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="2:4" ht="42.75">
+    <row r="34" spans="2:4" ht="43.75">
       <c r="B34" s="160"/>
       <c r="C34" s="135" t="s">
         <v>1572</v>
@@ -16947,7 +16947,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="35" spans="2:4" ht="57">
+    <row r="35" spans="2:4" ht="58.3">
       <c r="B35" s="160"/>
       <c r="C35" s="135" t="s">
         <v>76</v>
@@ -16956,7 +16956,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="2:4" ht="28.5">
+    <row r="36" spans="2:4" ht="43.75">
       <c r="B36" s="161"/>
       <c r="C36" s="136" t="s">
         <v>78</v>
@@ -16965,7 +16965,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="37" spans="2:4" ht="157.15" thickBot="1">
+    <row r="37" spans="2:4" ht="160.75" thickBot="1">
       <c r="B37" s="134" t="s">
         <v>80</v>
       </c>
@@ -16974,7 +16974,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="38" spans="2:4" ht="43.15" thickBot="1">
+    <row r="38" spans="2:4" ht="44.15" thickBot="1">
       <c r="B38" s="80" t="s">
         <v>82</v>
       </c>
@@ -17019,7 +17019,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="43" spans="2:4" ht="142.9" thickBot="1">
+    <row r="43" spans="2:4" ht="160.75" thickBot="1">
       <c r="B43" s="80" t="s">
         <v>92</v>
       </c>
@@ -17037,7 +17037,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="45" spans="2:4" ht="28.5">
+    <row r="45" spans="2:4" ht="29.15">
       <c r="B45" s="80" t="s">
         <v>96</v>
       </c>
@@ -17085,9 +17085,9 @@
       <selection activeCell="J35" sqref="A1:J35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.45"/>
   <cols>
-    <col min="1" max="1" width="3.1328125" customWidth="1"/>
+    <col min="1" max="1" width="3.15234375" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
   </cols>
   <sheetData>
@@ -17179,7 +17179,7 @@
       <c r="I8" s="171"/>
       <c r="J8" s="171"/>
     </row>
-    <row r="9" spans="2:10" ht="13.15">
+    <row r="9" spans="2:10">
       <c r="B9" s="2" t="s">
         <v>100</v>
       </c>
@@ -17194,7 +17194,7 @@
       <c r="I9" s="172"/>
       <c r="J9" s="172"/>
     </row>
-    <row r="10" spans="2:10" ht="13.15">
+    <row r="10" spans="2:10">
       <c r="B10" s="2" t="s">
         <v>102</v>
       </c>
@@ -17209,7 +17209,7 @@
       <c r="I10" s="172"/>
       <c r="J10" s="172"/>
     </row>
-    <row r="11" spans="2:10" ht="13.15">
+    <row r="11" spans="2:10">
       <c r="B11" s="2" t="s">
         <v>104</v>
       </c>
@@ -17222,8 +17222,8 @@
       <c r="I11" s="172"/>
       <c r="J11" s="172"/>
     </row>
-    <row r="12" spans="2:10" ht="13.15" thickBot="1"/>
-    <row r="13" spans="2:10" ht="13.9" thickTop="1" thickBot="1">
+    <row r="12" spans="2:10" ht="12.9" thickBot="1"/>
+    <row r="13" spans="2:10" ht="13.3" thickTop="1" thickBot="1">
       <c r="B13" s="3" t="s">
         <v>0</v>
       </c>
@@ -17238,7 +17238,7 @@
       <c r="I13" s="170"/>
       <c r="J13" s="170"/>
     </row>
-    <row r="14" spans="2:10" ht="13.9" thickTop="1" thickBot="1">
+    <row r="14" spans="2:10" ht="13.3" thickTop="1" thickBot="1">
       <c r="B14" s="4" t="s">
         <v>2</v>
       </c>
@@ -17253,7 +17253,7 @@
       <c r="I14" s="174"/>
       <c r="J14" s="174"/>
     </row>
-    <row r="15" spans="2:10" ht="13.9" thickTop="1" thickBot="1">
+    <row r="15" spans="2:10" ht="13.3" thickTop="1" thickBot="1">
       <c r="B15" s="5" t="s">
         <v>106</v>
       </c>
@@ -17268,7 +17268,7 @@
       <c r="I15" s="174"/>
       <c r="J15" s="174"/>
     </row>
-    <row r="16" spans="2:10" ht="13.9" thickTop="1" thickBot="1">
+    <row r="16" spans="2:10" ht="13.3" thickTop="1" thickBot="1">
       <c r="B16" s="5"/>
       <c r="C16" s="175"/>
       <c r="D16" s="175"/>
@@ -17279,7 +17279,7 @@
       <c r="I16" s="175"/>
       <c r="J16" s="175"/>
     </row>
-    <row r="17" spans="1:13" ht="13.9" thickTop="1" thickBot="1">
+    <row r="17" spans="1:13" ht="13.3" thickTop="1" thickBot="1">
       <c r="A17" s="1"/>
       <c r="B17" s="6"/>
       <c r="C17" s="175"/>
@@ -17294,7 +17294,7 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="1:13" ht="13.9" thickTop="1" thickBot="1">
+    <row r="18" spans="1:13" ht="13.3" thickTop="1" thickBot="1">
       <c r="B18" s="5"/>
       <c r="C18" s="174"/>
       <c r="D18" s="174"/>
@@ -17320,8 +17320,8 @@
       <c r="I19" s="175"/>
       <c r="J19" s="175"/>
     </row>
-    <row r="20" spans="1:13" ht="13.5" thickTop="1" thickBot="1"/>
-    <row r="21" spans="1:13" ht="13.9" thickTop="1" thickBot="1">
+    <row r="20" spans="1:13" ht="13.3" thickTop="1" thickBot="1"/>
+    <row r="21" spans="1:13" ht="13.3" thickTop="1" thickBot="1">
       <c r="B21" s="3" t="s">
         <v>110</v>
       </c>
@@ -17336,7 +17336,7 @@
       <c r="I21" s="170"/>
       <c r="J21" s="170"/>
     </row>
-    <row r="22" spans="1:13" ht="13.9" thickTop="1" thickBot="1">
+    <row r="22" spans="1:13" ht="13.75" thickTop="1" thickBot="1">
       <c r="B22" s="8"/>
       <c r="C22" s="174"/>
       <c r="D22" s="174"/>
@@ -17347,7 +17347,7 @@
       <c r="I22" s="174"/>
       <c r="J22" s="174"/>
     </row>
-    <row r="23" spans="1:13" ht="13.9" thickTop="1" thickBot="1">
+    <row r="23" spans="1:13" ht="13.75" thickTop="1" thickBot="1">
       <c r="B23" s="9"/>
       <c r="C23" s="174"/>
       <c r="D23" s="174"/>
@@ -17386,7 +17386,7 @@
       <c r="I25" s="175"/>
       <c r="J25" s="175"/>
     </row>
-    <row r="26" spans="1:13" ht="13.9" thickTop="1" thickBot="1">
+    <row r="26" spans="1:13" ht="13.75" thickTop="1" thickBot="1">
       <c r="B26" s="12" t="s">
         <v>112</v>
       </c>
@@ -17401,7 +17401,7 @@
       <c r="I26" s="174"/>
       <c r="J26" s="174"/>
     </row>
-    <row r="27" spans="1:13" ht="13.15" thickTop="1"/>
+    <row r="27" spans="1:13" ht="12.9" thickTop="1"/>
   </sheetData>
   <mergeCells count="17">
     <mergeCell ref="C22:J22"/>
@@ -17433,19 +17433,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16E684B6-2139-436B-862B-6D284F4F1B0E}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.45"/>
   <cols>
-    <col min="1" max="1" width="38.59765625" style="145" customWidth="1"/>
+    <col min="1" max="1" width="38.53515625" style="145" customWidth="1"/>
     <col min="2" max="2" width="58" style="145" customWidth="1"/>
-    <col min="3" max="3" width="59.3984375" style="145" customWidth="1"/>
-    <col min="4" max="16384" width="9.06640625" style="145"/>
+    <col min="3" max="3" width="59.3828125" style="145" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="145"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="13.15">
+    <row r="1" spans="1:3">
       <c r="A1" s="144" t="s">
         <v>1591</v>
       </c>
@@ -17708,43 +17708,43 @@
   <dimension ref="B1:AV25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AR26" sqref="AR26"/>
+      <selection pane="bottomRight" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="13.15"/>
+  <sheetFormatPr defaultColWidth="14.3828125" defaultRowHeight="12.9"/>
   <cols>
-    <col min="1" max="1" width="2.1328125" style="29" customWidth="1"/>
-    <col min="2" max="2" width="20.1328125" style="29" customWidth="1"/>
-    <col min="3" max="3" width="11.265625" style="29" customWidth="1"/>
-    <col min="4" max="5" width="30.73046875" style="16" customWidth="1"/>
-    <col min="6" max="10" width="14.86328125" style="29" customWidth="1"/>
-    <col min="11" max="11" width="18.3984375" style="29" customWidth="1"/>
-    <col min="12" max="14" width="14.86328125" style="29" customWidth="1"/>
-    <col min="15" max="15" width="28.3984375" style="29" customWidth="1"/>
-    <col min="16" max="16" width="39.1328125" style="29" customWidth="1"/>
-    <col min="17" max="18" width="15.73046875" style="29" customWidth="1"/>
-    <col min="19" max="19" width="30.73046875" style="29" customWidth="1"/>
-    <col min="20" max="20" width="15.86328125" style="29" customWidth="1"/>
-    <col min="21" max="21" width="30.73046875" style="29" customWidth="1"/>
-    <col min="22" max="22" width="15.73046875" style="29" customWidth="1"/>
-    <col min="23" max="23" width="30.73046875" style="29" customWidth="1"/>
-    <col min="24" max="25" width="15.73046875" style="29" customWidth="1"/>
-    <col min="26" max="26" width="30.73046875" style="29" customWidth="1"/>
-    <col min="27" max="27" width="15.73046875" style="29" customWidth="1"/>
-    <col min="28" max="28" width="25.265625" style="29" customWidth="1"/>
-    <col min="29" max="29" width="30.73046875" style="42" customWidth="1"/>
-    <col min="30" max="30" width="30.73046875" style="16" customWidth="1"/>
-    <col min="31" max="31" width="14.3984375" style="29"/>
-    <col min="32" max="32" width="25.3984375" style="29" customWidth="1"/>
-    <col min="33" max="33" width="27.73046875" style="29" customWidth="1"/>
-    <col min="34" max="34" width="14.3984375" style="29"/>
-    <col min="35" max="35" width="49.3984375" style="29" customWidth="1"/>
-    <col min="36" max="38" width="14.3984375" style="29"/>
-    <col min="39" max="39" width="24.73046875" style="29" customWidth="1"/>
-    <col min="40" max="16384" width="14.3984375" style="29"/>
+    <col min="1" max="1" width="2.15234375" style="29" customWidth="1"/>
+    <col min="2" max="2" width="20.15234375" style="29" customWidth="1"/>
+    <col min="3" max="3" width="11.3046875" style="29" customWidth="1"/>
+    <col min="4" max="5" width="30.69140625" style="16" customWidth="1"/>
+    <col min="6" max="10" width="14.84375" style="29" customWidth="1"/>
+    <col min="11" max="11" width="18.3828125" style="29" customWidth="1"/>
+    <col min="12" max="14" width="14.84375" style="29" customWidth="1"/>
+    <col min="15" max="15" width="28.3828125" style="29" customWidth="1"/>
+    <col min="16" max="16" width="39.15234375" style="29" customWidth="1"/>
+    <col min="17" max="18" width="15.69140625" style="29" customWidth="1"/>
+    <col min="19" max="19" width="30.69140625" style="29" customWidth="1"/>
+    <col min="20" max="20" width="15.84375" style="29" customWidth="1"/>
+    <col min="21" max="21" width="30.69140625" style="29" customWidth="1"/>
+    <col min="22" max="22" width="15.69140625" style="29" customWidth="1"/>
+    <col min="23" max="23" width="30.69140625" style="29" customWidth="1"/>
+    <col min="24" max="25" width="15.69140625" style="29" customWidth="1"/>
+    <col min="26" max="26" width="30.69140625" style="29" customWidth="1"/>
+    <col min="27" max="27" width="15.69140625" style="29" customWidth="1"/>
+    <col min="28" max="28" width="25.3046875" style="29" customWidth="1"/>
+    <col min="29" max="29" width="30.69140625" style="42" customWidth="1"/>
+    <col min="30" max="30" width="30.69140625" style="16" customWidth="1"/>
+    <col min="31" max="31" width="14.3828125" style="29"/>
+    <col min="32" max="32" width="25.3828125" style="29" customWidth="1"/>
+    <col min="33" max="33" width="27.69140625" style="29" customWidth="1"/>
+    <col min="34" max="34" width="14.3828125" style="29"/>
+    <col min="35" max="35" width="49.3828125" style="29" customWidth="1"/>
+    <col min="36" max="38" width="14.3828125" style="29"/>
+    <col min="39" max="39" width="24.69140625" style="29" customWidth="1"/>
+    <col min="40" max="16384" width="14.3828125" style="29"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:48" ht="30" customHeight="1">
@@ -19718,57 +19718,57 @@
   </sheetPr>
   <dimension ref="B1:AY65"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="7" ySplit="2" topLeftCell="AT58" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="7" ySplit="2" topLeftCell="AH46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AU64" sqref="AU64"/>
+      <selection pane="bottomRight" activeCell="AH52" sqref="AH52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="13.15"/>
+  <sheetFormatPr defaultColWidth="14.3828125" defaultRowHeight="12.9"/>
   <cols>
     <col min="1" max="1" width="4" style="29" customWidth="1"/>
-    <col min="2" max="2" width="14.3984375" style="29"/>
-    <col min="3" max="3" width="18.3984375" style="29" customWidth="1"/>
-    <col min="4" max="4" width="30.73046875" style="16" customWidth="1"/>
-    <col min="5" max="5" width="20.86328125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="14.3828125" style="29"/>
+    <col min="3" max="3" width="18.3828125" style="29" customWidth="1"/>
+    <col min="4" max="4" width="30.69140625" style="16" customWidth="1"/>
+    <col min="5" max="5" width="20.84375" style="16" customWidth="1"/>
     <col min="6" max="6" width="13" style="29" customWidth="1"/>
-    <col min="7" max="7" width="8.73046875" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.1328125" style="29" customWidth="1"/>
-    <col min="9" max="9" width="15.3984375" style="29" customWidth="1"/>
-    <col min="10" max="11" width="18.86328125" style="29" customWidth="1"/>
-    <col min="12" max="13" width="22.1328125" style="29" customWidth="1"/>
-    <col min="14" max="14" width="18.73046875" style="29" customWidth="1"/>
-    <col min="15" max="16" width="23.3984375" style="29" customWidth="1"/>
-    <col min="17" max="17" width="15.73046875" style="16" customWidth="1"/>
-    <col min="18" max="18" width="15.73046875" style="61" customWidth="1"/>
-    <col min="19" max="19" width="30.73046875" style="16" customWidth="1"/>
-    <col min="20" max="20" width="15.73046875" style="16" customWidth="1"/>
-    <col min="21" max="21" width="30.73046875" style="16" customWidth="1"/>
-    <col min="22" max="22" width="15.73046875" style="16" customWidth="1"/>
-    <col min="23" max="23" width="30.73046875" style="16" customWidth="1"/>
-    <col min="24" max="24" width="15.73046875" style="16" customWidth="1"/>
-    <col min="25" max="25" width="15.73046875" style="61" customWidth="1"/>
-    <col min="26" max="26" width="30.73046875" style="16" customWidth="1"/>
-    <col min="27" max="27" width="15.73046875" style="16" customWidth="1"/>
-    <col min="28" max="28" width="30.73046875" style="16" customWidth="1"/>
-    <col min="29" max="29" width="15.73046875" style="16" customWidth="1"/>
-    <col min="30" max="30" width="30.73046875" style="16" customWidth="1"/>
-    <col min="31" max="31" width="11.1328125" style="29" customWidth="1"/>
-    <col min="32" max="32" width="17.3984375" style="29" customWidth="1"/>
-    <col min="33" max="33" width="20.73046875" style="29" customWidth="1"/>
-    <col min="34" max="34" width="14.3984375" style="29"/>
-    <col min="35" max="35" width="21.73046875" style="29" customWidth="1"/>
-    <col min="36" max="37" width="14.3984375" style="29"/>
-    <col min="38" max="38" width="60.86328125" style="29" customWidth="1"/>
-    <col min="39" max="41" width="14.3984375" style="29"/>
-    <col min="42" max="42" width="33.86328125" style="29" customWidth="1"/>
-    <col min="43" max="46" width="14.3984375" style="29"/>
-    <col min="47" max="47" width="53.86328125" style="29" customWidth="1"/>
-    <col min="48" max="48" width="17.73046875" style="29" customWidth="1"/>
-    <col min="49" max="49" width="23.3984375" style="29" customWidth="1"/>
-    <col min="50" max="50" width="21.73046875" style="29" customWidth="1"/>
-    <col min="51" max="16384" width="14.3984375" style="29"/>
+    <col min="7" max="7" width="8.69140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.15234375" style="29" customWidth="1"/>
+    <col min="9" max="9" width="15.3828125" style="29" customWidth="1"/>
+    <col min="10" max="11" width="18.84375" style="29" customWidth="1"/>
+    <col min="12" max="13" width="22.15234375" style="29" customWidth="1"/>
+    <col min="14" max="14" width="18.69140625" style="29" customWidth="1"/>
+    <col min="15" max="16" width="23.3828125" style="29" customWidth="1"/>
+    <col min="17" max="17" width="15.69140625" style="16" customWidth="1"/>
+    <col min="18" max="18" width="15.69140625" style="61" customWidth="1"/>
+    <col min="19" max="19" width="30.69140625" style="16" customWidth="1"/>
+    <col min="20" max="20" width="15.69140625" style="16" customWidth="1"/>
+    <col min="21" max="21" width="30.69140625" style="16" customWidth="1"/>
+    <col min="22" max="22" width="15.69140625" style="16" customWidth="1"/>
+    <col min="23" max="23" width="30.69140625" style="16" customWidth="1"/>
+    <col min="24" max="24" width="15.69140625" style="16" customWidth="1"/>
+    <col min="25" max="25" width="15.69140625" style="61" customWidth="1"/>
+    <col min="26" max="26" width="30.69140625" style="16" customWidth="1"/>
+    <col min="27" max="27" width="15.69140625" style="16" customWidth="1"/>
+    <col min="28" max="28" width="30.69140625" style="16" customWidth="1"/>
+    <col min="29" max="29" width="15.69140625" style="16" customWidth="1"/>
+    <col min="30" max="30" width="30.69140625" style="16" customWidth="1"/>
+    <col min="31" max="31" width="11.15234375" style="29" customWidth="1"/>
+    <col min="32" max="32" width="17.3828125" style="29" customWidth="1"/>
+    <col min="33" max="33" width="20.69140625" style="29" customWidth="1"/>
+    <col min="34" max="34" width="14.3828125" style="29"/>
+    <col min="35" max="35" width="21.69140625" style="29" customWidth="1"/>
+    <col min="36" max="37" width="14.3828125" style="29"/>
+    <col min="38" max="38" width="60.84375" style="29" customWidth="1"/>
+    <col min="39" max="41" width="14.3828125" style="29"/>
+    <col min="42" max="42" width="33.84375" style="29" customWidth="1"/>
+    <col min="43" max="46" width="14.3828125" style="29"/>
+    <col min="47" max="47" width="53.84375" style="29" customWidth="1"/>
+    <col min="48" max="48" width="17.69140625" style="29" customWidth="1"/>
+    <col min="49" max="49" width="23.3828125" style="29" customWidth="1"/>
+    <col min="50" max="50" width="21.69140625" style="29" customWidth="1"/>
+    <col min="51" max="16384" width="14.3828125" style="29"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:51" ht="30" customHeight="1">
@@ -26655,35 +26655,35 @@
       <selection pane="bottomRight" activeCell="AN4" sqref="AN4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="13.15"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.45"/>
   <cols>
-    <col min="1" max="1" width="19.265625" style="78" customWidth="1"/>
-    <col min="2" max="2" width="12.265625" style="35" customWidth="1"/>
-    <col min="3" max="3" width="30.73046875" style="35" customWidth="1"/>
-    <col min="4" max="4" width="70.86328125" style="35" customWidth="1"/>
-    <col min="5" max="5" width="12.86328125" style="35" customWidth="1"/>
-    <col min="6" max="6" width="8.86328125" style="35"/>
-    <col min="7" max="7" width="10.1328125" style="35" customWidth="1"/>
-    <col min="8" max="8" width="10.3984375" style="35" customWidth="1"/>
-    <col min="9" max="9" width="8.86328125" style="35"/>
-    <col min="10" max="10" width="24.73046875" style="35" customWidth="1"/>
-    <col min="11" max="12" width="8.86328125" style="35"/>
-    <col min="13" max="13" width="14.3984375" style="35" customWidth="1"/>
-    <col min="14" max="14" width="28.73046875" style="35" customWidth="1"/>
-    <col min="15" max="15" width="60.73046875" style="35" customWidth="1"/>
-    <col min="16" max="17" width="15.73046875" style="35" customWidth="1"/>
-    <col min="18" max="18" width="30.73046875" style="35" customWidth="1"/>
-    <col min="19" max="19" width="15.73046875" style="35" customWidth="1"/>
-    <col min="20" max="20" width="30.73046875" style="35" customWidth="1"/>
-    <col min="21" max="21" width="15.73046875" style="35" customWidth="1"/>
-    <col min="22" max="22" width="30.73046875" style="35" customWidth="1"/>
-    <col min="23" max="24" width="15.73046875" style="35" customWidth="1"/>
-    <col min="25" max="25" width="30.73046875" style="35" customWidth="1"/>
-    <col min="26" max="26" width="15.73046875" style="35" customWidth="1"/>
-    <col min="27" max="27" width="30.73046875" style="35" customWidth="1"/>
-    <col min="28" max="28" width="15.73046875" style="35" customWidth="1"/>
-    <col min="29" max="29" width="30.73046875" style="35" customWidth="1"/>
-    <col min="30" max="16384" width="8.86328125" style="35"/>
+    <col min="1" max="1" width="19.3046875" style="78" customWidth="1"/>
+    <col min="2" max="2" width="12.3046875" style="35" customWidth="1"/>
+    <col min="3" max="3" width="30.69140625" style="35" customWidth="1"/>
+    <col min="4" max="4" width="70.84375" style="35" customWidth="1"/>
+    <col min="5" max="5" width="12.84375" style="35" customWidth="1"/>
+    <col min="6" max="6" width="8.84375" style="35"/>
+    <col min="7" max="7" width="10.15234375" style="35" customWidth="1"/>
+    <col min="8" max="8" width="10.3828125" style="35" customWidth="1"/>
+    <col min="9" max="9" width="8.84375" style="35"/>
+    <col min="10" max="10" width="24.69140625" style="35" customWidth="1"/>
+    <col min="11" max="12" width="8.84375" style="35"/>
+    <col min="13" max="13" width="14.3828125" style="35" customWidth="1"/>
+    <col min="14" max="14" width="28.69140625" style="35" customWidth="1"/>
+    <col min="15" max="15" width="60.69140625" style="35" customWidth="1"/>
+    <col min="16" max="17" width="15.69140625" style="35" customWidth="1"/>
+    <col min="18" max="18" width="30.69140625" style="35" customWidth="1"/>
+    <col min="19" max="19" width="15.69140625" style="35" customWidth="1"/>
+    <col min="20" max="20" width="30.69140625" style="35" customWidth="1"/>
+    <col min="21" max="21" width="15.69140625" style="35" customWidth="1"/>
+    <col min="22" max="22" width="30.69140625" style="35" customWidth="1"/>
+    <col min="23" max="24" width="15.69140625" style="35" customWidth="1"/>
+    <col min="25" max="25" width="30.69140625" style="35" customWidth="1"/>
+    <col min="26" max="26" width="15.69140625" style="35" customWidth="1"/>
+    <col min="27" max="27" width="30.69140625" style="35" customWidth="1"/>
+    <col min="28" max="28" width="15.69140625" style="35" customWidth="1"/>
+    <col min="29" max="29" width="30.69140625" style="35" customWidth="1"/>
+    <col min="30" max="16384" width="8.84375" style="35"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:45" ht="30" customHeight="1">
@@ -28005,49 +28005,49 @@
       <selection pane="bottomRight" activeCell="AR25" sqref="AR25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="13.15"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.9"/>
   <cols>
-    <col min="1" max="1" width="10.3984375" style="29" customWidth="1"/>
-    <col min="2" max="2" width="12.265625" style="29" customWidth="1"/>
-    <col min="3" max="3" width="30.73046875" style="29" customWidth="1"/>
-    <col min="4" max="4" width="10.265625" style="16" customWidth="1"/>
-    <col min="5" max="5" width="10.86328125" style="29" customWidth="1"/>
-    <col min="6" max="6" width="17.86328125" style="29" customWidth="1"/>
-    <col min="7" max="7" width="32.86328125" style="29" customWidth="1"/>
-    <col min="8" max="8" width="9.1328125" style="29"/>
-    <col min="9" max="9" width="16.3984375" style="29" customWidth="1"/>
-    <col min="10" max="10" width="24.73046875" style="29" customWidth="1"/>
-    <col min="11" max="12" width="9.1328125" style="29"/>
-    <col min="13" max="13" width="23.86328125" style="16" customWidth="1"/>
-    <col min="14" max="14" width="28.73046875" style="29" customWidth="1"/>
-    <col min="15" max="15" width="42.3984375" style="29" customWidth="1"/>
-    <col min="16" max="16" width="15.73046875" style="28" customWidth="1"/>
-    <col min="17" max="17" width="15.73046875" style="61" customWidth="1"/>
-    <col min="18" max="18" width="30.73046875" style="16" customWidth="1"/>
-    <col min="19" max="19" width="15.73046875" style="16" customWidth="1"/>
-    <col min="20" max="20" width="30.73046875" style="16" customWidth="1"/>
-    <col min="21" max="21" width="15.73046875" style="16" customWidth="1"/>
-    <col min="22" max="22" width="30.73046875" style="16" customWidth="1"/>
-    <col min="23" max="23" width="15.73046875" style="16" customWidth="1"/>
-    <col min="24" max="24" width="15.73046875" style="61" customWidth="1"/>
-    <col min="25" max="25" width="30.73046875" style="16" customWidth="1"/>
-    <col min="26" max="26" width="15.73046875" style="16" customWidth="1"/>
-    <col min="27" max="27" width="30.73046875" style="16" customWidth="1"/>
-    <col min="28" max="28" width="15.73046875" style="16" customWidth="1"/>
-    <col min="29" max="29" width="30.73046875" style="16" customWidth="1"/>
-    <col min="30" max="30" width="6.265625" style="29" customWidth="1"/>
-    <col min="31" max="31" width="9.265625" style="29" customWidth="1"/>
-    <col min="32" max="32" width="8.265625" style="16" customWidth="1"/>
-    <col min="33" max="33" width="9.1328125" style="29"/>
+    <col min="1" max="1" width="10.3828125" style="29" customWidth="1"/>
+    <col min="2" max="2" width="12.3046875" style="29" customWidth="1"/>
+    <col min="3" max="3" width="30.69140625" style="29" customWidth="1"/>
+    <col min="4" max="4" width="10.3046875" style="16" customWidth="1"/>
+    <col min="5" max="5" width="10.84375" style="29" customWidth="1"/>
+    <col min="6" max="6" width="17.84375" style="29" customWidth="1"/>
+    <col min="7" max="7" width="32.84375" style="29" customWidth="1"/>
+    <col min="8" max="8" width="9.15234375" style="29"/>
+    <col min="9" max="9" width="16.3828125" style="29" customWidth="1"/>
+    <col min="10" max="10" width="24.69140625" style="29" customWidth="1"/>
+    <col min="11" max="12" width="9.15234375" style="29"/>
+    <col min="13" max="13" width="23.84375" style="16" customWidth="1"/>
+    <col min="14" max="14" width="28.69140625" style="29" customWidth="1"/>
+    <col min="15" max="15" width="42.3828125" style="29" customWidth="1"/>
+    <col min="16" max="16" width="15.69140625" style="28" customWidth="1"/>
+    <col min="17" max="17" width="15.69140625" style="61" customWidth="1"/>
+    <col min="18" max="18" width="30.69140625" style="16" customWidth="1"/>
+    <col min="19" max="19" width="15.69140625" style="16" customWidth="1"/>
+    <col min="20" max="20" width="30.69140625" style="16" customWidth="1"/>
+    <col min="21" max="21" width="15.69140625" style="16" customWidth="1"/>
+    <col min="22" max="22" width="30.69140625" style="16" customWidth="1"/>
+    <col min="23" max="23" width="15.69140625" style="16" customWidth="1"/>
+    <col min="24" max="24" width="15.69140625" style="61" customWidth="1"/>
+    <col min="25" max="25" width="30.69140625" style="16" customWidth="1"/>
+    <col min="26" max="26" width="15.69140625" style="16" customWidth="1"/>
+    <col min="27" max="27" width="30.69140625" style="16" customWidth="1"/>
+    <col min="28" max="28" width="15.69140625" style="16" customWidth="1"/>
+    <col min="29" max="29" width="30.69140625" style="16" customWidth="1"/>
+    <col min="30" max="30" width="6.3046875" style="29" customWidth="1"/>
+    <col min="31" max="31" width="9.3046875" style="29" customWidth="1"/>
+    <col min="32" max="32" width="8.3046875" style="16" customWidth="1"/>
+    <col min="33" max="33" width="9.15234375" style="29"/>
     <col min="34" max="34" width="27" style="29" customWidth="1"/>
     <col min="35" max="35" width="14" style="29" customWidth="1"/>
-    <col min="36" max="36" width="9.1328125" style="29"/>
+    <col min="36" max="36" width="9.15234375" style="29"/>
     <col min="37" max="37" width="56" style="29" customWidth="1"/>
-    <col min="38" max="39" width="9.1328125" style="29"/>
+    <col min="38" max="39" width="9.15234375" style="29"/>
     <col min="40" max="40" width="20" style="29" customWidth="1"/>
-    <col min="41" max="43" width="9.1328125" style="29"/>
-    <col min="44" max="44" width="49.73046875" style="29" customWidth="1"/>
-    <col min="45" max="16384" width="9.1328125" style="29"/>
+    <col min="41" max="43" width="9.15234375" style="29"/>
+    <col min="44" max="44" width="49.69140625" style="29" customWidth="1"/>
+    <col min="45" max="16384" width="9.15234375" style="29"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48" ht="30" customHeight="1">
@@ -32973,11 +32973,11 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="1" width="4.3984375" style="90" customWidth="1"/>
+    <col min="1" max="1" width="4.3828125" style="90" customWidth="1"/>
     <col min="2" max="2" width="100" style="93" customWidth="1"/>
-    <col min="3" max="16384" width="9.1328125" style="90"/>
+    <col min="3" max="16384" width="9.15234375" style="90"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="91" customFormat="1">
@@ -32997,7 +32997,7 @@
         <v>1566</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" ht="29.15">
       <c r="A4" s="90">
         <f>A3+1</f>
         <v>2</v>
@@ -33040,89 +33040,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="51983ca6-de84-41fa-9a65-1d08ee1009bc">
-      <UserInfo>
-        <DisplayName>RATANAPRAYUL, Natschja</DisplayName>
-        <AccountId>7</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Pete Christopher (Green Ink) (p.christopher@greenink.co.uk)</DisplayName>
-        <AccountId>26</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BARREIX ETCHEGOIMBERRY, Maria</DisplayName>
-        <AccountId>13</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>AMIN, Avni</DisplayName>
-        <AccountId>46</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>GARCIA MORENO ESTEVA, Claudia M.</DisplayName>
-        <AccountId>47</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>KIPRUTO, Hillary Kipchumba</DisplayName>
-        <AccountId>28</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>SEYDI, Aminata Binetou Wahebine</DisplayName>
-        <AccountId>61</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>TITI-OFEI, Regina</DisplayName>
-        <AccountId>62</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>COSMAS, Leonard</DisplayName>
-        <AccountId>63</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>AUSTIN, Marie-pierre</DisplayName>
-        <AccountId>80</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>JALANTI, Lauri</DisplayName>
-        <AccountId>81</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>EFIMOVA, Anjelika</DisplayName>
-        <AccountId>82</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>TAMRAT, Tigest</DisplayName>
-        <AccountId>21</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008A6DDC313EDC9A43B330D8B6305883A5" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8a49ef05ae535a507bc3e9747af69e28">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="73389989-ac93-4f39-a9f3-2949bbf25fcc" xmlns:ns3="51983ca6-de84-41fa-9a65-1d08ee1009bc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d5708882d0641db35f33240439156254" ns2:_="" ns3:_="">
     <xsd:import namespace="73389989-ac93-4f39-a9f3-2949bbf25fcc"/>
@@ -33333,25 +33250,90 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3641399-1C83-4230-9FA0-63883702B763}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5128250D-9B2C-4D86-9D99-709881CA8B0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="51983ca6-de84-41fa-9a65-1d08ee1009bc"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="51983ca6-de84-41fa-9a65-1d08ee1009bc">
+      <UserInfo>
+        <DisplayName>RATANAPRAYUL, Natschja</DisplayName>
+        <AccountId>7</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Pete Christopher (Green Ink) (p.christopher@greenink.co.uk)</DisplayName>
+        <AccountId>26</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BARREIX ETCHEGOIMBERRY, Maria</DisplayName>
+        <AccountId>13</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>AMIN, Avni</DisplayName>
+        <AccountId>46</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>GARCIA MORENO ESTEVA, Claudia M.</DisplayName>
+        <AccountId>47</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>KIPRUTO, Hillary Kipchumba</DisplayName>
+        <AccountId>28</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>SEYDI, Aminata Binetou Wahebine</DisplayName>
+        <AccountId>61</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>TITI-OFEI, Regina</DisplayName>
+        <AccountId>62</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>COSMAS, Leonard</DisplayName>
+        <AccountId>63</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>AUSTIN, Marie-pierre</DisplayName>
+        <AccountId>80</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>JALANTI, Lauri</DisplayName>
+        <AccountId>81</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>EFIMOVA, Anjelika</DisplayName>
+        <AccountId>82</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>TAMRAT, Tigest</DisplayName>
+        <AccountId>21</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38467C22-69D6-4596-9AF7-36CE3664857A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -33368,4 +33350,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3641399-1C83-4230-9FA0-63883702B763}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5128250D-9B2C-4D86-9D99-709881CA8B0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="51983ca6-de84-41fa-9a65-1d08ee1009bc"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>